<commit_message>
TA-01 / AdminScenario: Filteration of user
</commit_message>
<xml_diff>
--- a/tests/testscenarios.xlsx
+++ b/tests/testscenarios.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="204">
   <si>
     <t>Test Step</t>
   </si>
@@ -504,6 +504,87 @@
     <t>CREATEUSER_SUBMIT</t>
   </si>
   <si>
+    <t>USERCREATION_SUCCESSMESSAGE</t>
+  </si>
+  <si>
+    <t>User Automation User created successfully.</t>
+  </si>
+  <si>
+    <t>CREATEUSERMENU_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>TS33</t>
+  </si>
+  <si>
+    <t>TS34</t>
+  </si>
+  <si>
+    <t>TS35</t>
+  </si>
+  <si>
+    <t>TS36</t>
+  </si>
+  <si>
+    <t>TS37</t>
+  </si>
+  <si>
+    <t>FILTER_USERNAME</t>
+  </si>
+  <si>
+    <t>TS38</t>
+  </si>
+  <si>
+    <t>FILTER_BUTTON</t>
+  </si>
+  <si>
+    <t>partialLinkText</t>
+  </si>
+  <si>
+    <t>TS39</t>
+  </si>
+  <si>
+    <t>TS40</t>
+  </si>
+  <si>
+    <t>TS41</t>
+  </si>
+  <si>
+    <t>TS42</t>
+  </si>
+  <si>
+    <t>TS43</t>
+  </si>
+  <si>
+    <t>TS44</t>
+  </si>
+  <si>
+    <t>TS45</t>
+  </si>
+  <si>
+    <t>TS46</t>
+  </si>
+  <si>
+    <t>TS47</t>
+  </si>
+  <si>
+    <t>TS48</t>
+  </si>
+  <si>
+    <t>TS49</t>
+  </si>
+  <si>
+    <t>TS50</t>
+  </si>
+  <si>
+    <t>TS51</t>
+  </si>
+  <si>
+    <t>searchElement</t>
+  </si>
+  <si>
+    <t>FILTER_TABLE</t>
+  </si>
+  <si>
     <t>clicked on ADMIN_LINK</t>
   </si>
   <si>
@@ -529,6 +610,27 @@
   </si>
   <si>
     <t>clicked on CREATEUSER_SUBMIT</t>
+  </si>
+  <si>
+    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                 Error: The username is already in use.                    </t>
+  </si>
+  <si>
+    <t>clicked on CREATEUSERMENU_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>Typed AutomationUser into USERNAME_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t>Typed Auto123 into PASSWORD_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t>Typed AutomationUser into FILTER_USERNAME text box</t>
+  </si>
+  <si>
+    <t>clicked on FILTER_BUTTON</t>
+  </si>
+  <si>
+    <t>Found FILTER_TABLE</t>
   </si>
 </sst>
 </file>
@@ -989,7 +1091,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,7 +1959,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E22" r:id="rId72" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
+    <hyperlink ref="E22" r:id="rId86" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -2008,10 +2110,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB88CC8-F150-4CAF-B716-3BC4266F1F49}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,7 +2305,7 @@
         <v>88</v>
       </c>
       <c r="G9" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2243,7 +2345,7 @@
         <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2262,7 +2364,7 @@
         <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>163</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2285,7 +2387,7 @@
         <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2308,7 +2410,7 @@
         <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2331,7 +2433,7 @@
         <v>88</v>
       </c>
       <c r="G15" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2354,7 +2456,7 @@
         <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2377,7 +2479,7 @@
         <v>88</v>
       </c>
       <c r="G17" t="s">
-        <v>168</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2398,12 +2500,535 @@
         <v>88</v>
       </c>
       <c r="G18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F33" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" t="s">
+        <v>88</v>
+      </c>
+      <c r="G34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" t="s">
+        <v>88</v>
+      </c>
+      <c r="G35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" t="s">
+        <v>88</v>
+      </c>
+      <c r="G36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" t="s">
+        <v>88</v>
+      </c>
+      <c r="G38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
         <v>169</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F41" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" t="s">
+        <v>88</v>
+      </c>
+      <c r="G42" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G43" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId72" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
+    <hyperlink ref="E15" r:id="rId86" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
@@ -2414,8 +3039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DBC0D3-CECE-4FBE-AFB4-B36031420D19}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TA-01/EDIT - DELETE Scenarios
</commit_message>
<xml_diff>
--- a/tests/testscenarios.xlsx
+++ b/tests/testscenarios.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="231">
   <si>
     <t>Test Step</t>
   </si>
@@ -387,202 +387,265 @@
     <t>Typed Vishak.Nair into USERNAME_TEXTBOX text box</t>
   </si>
   <si>
+    <t xml:space="preserve">User Settings </t>
+  </si>
+  <si>
+    <t>USER_SETTINGS</t>
+  </si>
+  <si>
+    <t>verifyElement</t>
+  </si>
+  <si>
+    <t>OLD_PASSWORD</t>
+  </si>
+  <si>
+    <t>NEW_PASSWORD</t>
+  </si>
+  <si>
+    <t>CONFIRM_PASSWORD</t>
+  </si>
+  <si>
+    <t>UPDATE_BUTTON</t>
+  </si>
+  <si>
+    <t>Interface2</t>
+  </si>
+  <si>
+    <t>USER_NAME_SETTINGS</t>
+  </si>
+  <si>
+    <t>LOGIN_ERRORMSG</t>
+  </si>
+  <si>
+    <t>Login Error: The username/password you provided were incorrect.</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>ADMIN_LINK</t>
+  </si>
+  <si>
+    <t>getTextContent</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>clicked on SETTINGS_LINK</t>
+  </si>
+  <si>
+    <t>Element present : USER_SETTINGS</t>
+  </si>
+  <si>
+    <t>Element present : vishak.nair</t>
+  </si>
+  <si>
+    <t>Typed Interface1 into OLD_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Typed Interface2 into NEW_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Typed Interface2 into CONFIRM_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>clicked on UPDATE_BUTTON</t>
+  </si>
+  <si>
+    <t>clicked on LOGOUT_LINK</t>
+  </si>
+  <si>
+    <t>clear the field  PASSWORD_TEXTBOX</t>
+  </si>
+  <si>
+    <t>Typed Interface2 into PASSWORD_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t>Element present : Login Error: The username/password you provided were incorrect.</t>
+  </si>
+  <si>
+    <t>CREATE_NEWUSER</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>CREATEUSER_USERNAME</t>
+  </si>
+  <si>
+    <t>AutomationUser</t>
+  </si>
+  <si>
+    <t>Create User</t>
+  </si>
+  <si>
+    <t>CREATEUSER_TITLE</t>
+  </si>
+  <si>
+    <t>CREATEUSER_EMAIL</t>
+  </si>
+  <si>
+    <t>CREATEUSER_PASSWORD</t>
+  </si>
+  <si>
+    <t>CREATEUSER_CONFIRMPASSWORD</t>
+  </si>
+  <si>
+    <t>nandini.rajaram@interfacesys.com</t>
+  </si>
+  <si>
+    <t>Auto123</t>
+  </si>
+  <si>
+    <t>CREATEUSER_SUBMIT</t>
+  </si>
+  <si>
+    <t>USERCREATION_SUCCESSMESSAGE</t>
+  </si>
+  <si>
+    <t>User Automation User created successfully.</t>
+  </si>
+  <si>
+    <t>CREATEUSERMENU_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>TS33</t>
+  </si>
+  <si>
+    <t>TS34</t>
+  </si>
+  <si>
+    <t>TS35</t>
+  </si>
+  <si>
+    <t>TS36</t>
+  </si>
+  <si>
+    <t>TS37</t>
+  </si>
+  <si>
+    <t>FILTER_USERNAME</t>
+  </si>
+  <si>
+    <t>TS38</t>
+  </si>
+  <si>
+    <t>FILTER_BUTTON</t>
+  </si>
+  <si>
+    <t>partialLinkText</t>
+  </si>
+  <si>
+    <t>TS39</t>
+  </si>
+  <si>
+    <t>TS40</t>
+  </si>
+  <si>
+    <t>TS41</t>
+  </si>
+  <si>
+    <t>TS42</t>
+  </si>
+  <si>
+    <t>TS43</t>
+  </si>
+  <si>
+    <t>TS44</t>
+  </si>
+  <si>
+    <t>TS45</t>
+  </si>
+  <si>
+    <t>TS46</t>
+  </si>
+  <si>
+    <t>TS47</t>
+  </si>
+  <si>
+    <t>TS48</t>
+  </si>
+  <si>
+    <t>TS49</t>
+  </si>
+  <si>
+    <t>TS50</t>
+  </si>
+  <si>
+    <t>TS51</t>
+  </si>
+  <si>
+    <t>searchElement</t>
+  </si>
+  <si>
+    <t>FILTER_TABLE</t>
+  </si>
+  <si>
     <t>clicked on CHANGECOMPANY_LINK</t>
   </si>
   <si>
-    <t xml:space="preserve">User Settings </t>
-  </si>
-  <si>
-    <t>USER_SETTINGS</t>
-  </si>
-  <si>
-    <t>verifyElement</t>
-  </si>
-  <si>
-    <t>OLD_PASSWORD</t>
-  </si>
-  <si>
-    <t>NEW_PASSWORD</t>
-  </si>
-  <si>
-    <t>CONFIRM_PASSWORD</t>
-  </si>
-  <si>
-    <t>UPDATE_BUTTON</t>
-  </si>
-  <si>
-    <t>Interface2</t>
-  </si>
-  <si>
-    <t>USER_NAME_SETTINGS</t>
-  </si>
-  <si>
-    <t>LOGIN_ERRORMSG</t>
-  </si>
-  <si>
-    <t>Login Error: The username/password you provided were incorrect.</t>
-  </si>
-  <si>
-    <t>clear</t>
-  </si>
-  <si>
-    <t>ADMIN_LINK</t>
-  </si>
-  <si>
-    <t>getTextContent</t>
-  </si>
-  <si>
-    <t>Administration</t>
-  </si>
-  <si>
-    <t>clicked on SETTINGS_LINK</t>
-  </si>
-  <si>
-    <t>Element present : USER_SETTINGS</t>
-  </si>
-  <si>
-    <t>Element present : vishak.nair</t>
-  </si>
-  <si>
-    <t>Typed Interface1 into OLD_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Typed Interface2 into NEW_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Typed Interface2 into CONFIRM_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>clicked on UPDATE_BUTTON</t>
-  </si>
-  <si>
-    <t>clicked on LOGOUT_LINK</t>
-  </si>
-  <si>
-    <t>clear the field  PASSWORD_TEXTBOX</t>
-  </si>
-  <si>
-    <t>Typed Interface2 into PASSWORD_TEXTBOX text box</t>
-  </si>
-  <si>
-    <t>Element present : Login Error: The username/password you provided were incorrect.</t>
-  </si>
-  <si>
-    <t>CREATE_NEWUSER</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>CREATEUSER_USERNAME</t>
-  </si>
-  <si>
-    <t>AutomationUser</t>
-  </si>
-  <si>
-    <t>Create User</t>
-  </si>
-  <si>
-    <t>CREATEUSER_TITLE</t>
-  </si>
-  <si>
-    <t>CREATEUSER_EMAIL</t>
-  </si>
-  <si>
-    <t>CREATEUSER_PASSWORD</t>
-  </si>
-  <si>
-    <t>CREATEUSER_CONFIRMPASSWORD</t>
-  </si>
-  <si>
-    <t>nandini.rajaram@interfacesys.com</t>
-  </si>
-  <si>
-    <t>Auto123</t>
-  </si>
-  <si>
-    <t>CREATEUSER_SUBMIT</t>
-  </si>
-  <si>
-    <t>USERCREATION_SUCCESSMESSAGE</t>
-  </si>
-  <si>
-    <t>User Automation User created successfully.</t>
-  </si>
-  <si>
-    <t>CREATEUSERMENU_CLOSEBUTTON</t>
-  </si>
-  <si>
-    <t>TS33</t>
-  </si>
-  <si>
-    <t>TS34</t>
-  </si>
-  <si>
-    <t>TS35</t>
-  </si>
-  <si>
-    <t>TS36</t>
-  </si>
-  <si>
-    <t>TS37</t>
-  </si>
-  <si>
-    <t>FILTER_USERNAME</t>
-  </si>
-  <si>
-    <t>TS38</t>
-  </si>
-  <si>
-    <t>FILTER_BUTTON</t>
-  </si>
-  <si>
-    <t>partialLinkText</t>
-  </si>
-  <si>
-    <t>TS39</t>
-  </si>
-  <si>
-    <t>TS40</t>
-  </si>
-  <si>
-    <t>TS41</t>
-  </si>
-  <si>
-    <t>TS42</t>
-  </si>
-  <si>
-    <t>TS43</t>
-  </si>
-  <si>
-    <t>TS44</t>
-  </si>
-  <si>
-    <t>TS45</t>
-  </si>
-  <si>
-    <t>TS46</t>
-  </si>
-  <si>
-    <t>TS47</t>
-  </si>
-  <si>
-    <t>TS48</t>
-  </si>
-  <si>
-    <t>TS49</t>
-  </si>
-  <si>
-    <t>TS50</t>
-  </si>
-  <si>
-    <t>TS51</t>
-  </si>
-  <si>
-    <t>searchElement</t>
-  </si>
-  <si>
-    <t>FILTER_TABLE</t>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>Waiting for 5000 millisecond  text box to be present</t>
+  </si>
+  <si>
+    <t>TS52</t>
+  </si>
+  <si>
+    <t>EDITAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>TS53</t>
+  </si>
+  <si>
+    <t>TS54</t>
+  </si>
+  <si>
+    <t>EDITUSER_TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit User </t>
+  </si>
+  <si>
+    <t>TS55</t>
+  </si>
+  <si>
+    <t>ADMINROLE_CHECKBOX</t>
+  </si>
+  <si>
+    <t>TS56</t>
+  </si>
+  <si>
+    <t>UPDATEBUTTON_EDITSCREEN</t>
+  </si>
+  <si>
+    <t>TS57</t>
+  </si>
+  <si>
+    <t>TS58</t>
+  </si>
+  <si>
+    <t>EDITSCREEN_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>TS59</t>
+  </si>
+  <si>
+    <t>TS60</t>
+  </si>
+  <si>
+    <t>DELETEAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>accept alert</t>
+  </si>
+  <si>
+    <t>TS61</t>
+  </si>
+  <si>
+    <t>TS62</t>
   </si>
   <si>
     <t>clicked on ADMIN_LINK</t>
@@ -612,7 +675,7 @@
     <t>clicked on CREATEUSER_SUBMIT</t>
   </si>
   <si>
-    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                 Error: The username is already in use.                    </t>
+    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                 Error: The username is already in use.</t>
   </si>
   <si>
     <t>clicked on CREATEUSERMENU_CLOSEBUTTON</t>
@@ -631,6 +694,24 @@
   </si>
   <si>
     <t>Found FILTER_TABLE</t>
+  </si>
+  <si>
+    <t>clicked on EDITAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>Element present : Edit User</t>
+  </si>
+  <si>
+    <t>clicked on ADMINROLE_CHECKBOX</t>
+  </si>
+  <si>
+    <t>clicked on UPDATEBUTTON_EDITSCREEN</t>
+  </si>
+  <si>
+    <t>clicked on EDITSCREEN_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>clicked on DELETEAUTOMATIONUSER</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1105,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1156,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
         <v>118</v>
@@ -1091,7 +1172,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,7 +1344,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I2"/>
+      <selection activeCell="A26" sqref="A26:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,7 +2040,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E22" r:id="rId86" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
+    <hyperlink ref="E22" r:id="rId292" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1968,15 +2049,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C24C14-A866-4140-B688-97F68D23BE6D}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="27.5703125" hidden="false" bestFit="false" style="0"/>
+    <col min="4" max="4" width="20.140625" hidden="false" bestFit="false" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2063,7 +2145,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -2084,36 +2166,76 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" t="s">
-        <v>122</v>
-      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB88CC8-F150-4CAF-B716-3BC4266F1F49}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2125,7 +2247,7 @@
     <col min="5" max="5" width="16.85546875" hidden="false" bestFit="false" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2142,7 +2264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2161,7 +2283,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2184,7 +2306,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2207,7 +2329,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2228,7 +2350,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -2247,7 +2369,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -2268,7 +2390,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2287,7 +2409,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -2295,7 +2417,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
@@ -2305,10 +2427,10 @@
         <v>88</v>
       </c>
       <c r="G9" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -2327,7 +2449,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -2335,7 +2457,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
@@ -2345,10 +2467,10 @@
         <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -2358,16 +2480,16 @@
         <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F12" t="s">
         <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -2375,22 +2497,22 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F13" t="s">
         <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -2398,22 +2520,22 @@
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F14" t="s">
         <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -2421,22 +2543,22 @@
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F15" t="s">
         <v>88</v>
       </c>
       <c r="G15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -2444,22 +2566,22 @@
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F16" t="s">
         <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
@@ -2467,22 +2589,22 @@
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F17" t="s">
         <v>88</v>
       </c>
       <c r="G17" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
@@ -2490,7 +2612,7 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
@@ -2500,10 +2622,10 @@
         <v>88</v>
       </c>
       <c r="G18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -2511,22 +2633,22 @@
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="F19" t="s">
         <v>88</v>
       </c>
       <c r="G19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
@@ -2534,7 +2656,7 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>10</v>
@@ -2544,10 +2666,10 @@
         <v>88</v>
       </c>
       <c r="G20" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>83</v>
       </c>
@@ -2568,7 +2690,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>84</v>
       </c>
@@ -2587,7 +2709,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>85</v>
       </c>
@@ -2605,10 +2727,10 @@
         <v>88</v>
       </c>
       <c r="G23" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>86</v>
       </c>
@@ -2627,9 +2749,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -2641,18 +2763,18 @@
         <v>6</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F25" t="s">
         <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>9</v>
@@ -2664,18 +2786,18 @@
         <v>6</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F26" t="s">
         <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>9</v>
@@ -2694,9 +2816,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2713,9 +2835,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>11</v>
@@ -2734,9 +2856,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2753,9 +2875,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
@@ -2771,12 +2893,12 @@
         <v>88</v>
       </c>
       <c r="G31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2793,9 +2915,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>9</v>
@@ -2816,9 +2938,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>9</v>
@@ -2839,9 +2961,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>9</v>
@@ -2860,9 +2982,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2879,9 +3001,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>11</v>
@@ -2900,9 +3022,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2919,15 +3041,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>10</v>
@@ -2937,12 +3059,12 @@
         <v>88</v>
       </c>
       <c r="G39" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2959,38 +3081,38 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F41" t="s">
         <v>88</v>
       </c>
       <c r="G41" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>10</v>
@@ -3000,35 +3122,250 @@
         <v>88</v>
       </c>
       <c r="G42" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F43" t="s">
         <v>88</v>
       </c>
       <c r="G43" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>191</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" t="s">
+        <v>88</v>
+      </c>
+      <c r="G44" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" t="s">
+        <v>88</v>
+      </c>
+      <c r="G45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F46" t="s">
+        <v>88</v>
+      </c>
+      <c r="G46" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" t="s">
+        <v>88</v>
+      </c>
+      <c r="G47" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" t="s">
+        <v>88</v>
+      </c>
+      <c r="G48" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" t="s">
+        <v>88</v>
+      </c>
+      <c r="G49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" t="s">
+        <v>88</v>
+      </c>
+      <c r="G50" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" t="s">
+        <v>88</v>
+      </c>
+      <c r="G51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" t="s">
+        <v>88</v>
+      </c>
+      <c r="G52" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" t="s">
+        <v>88</v>
+      </c>
+      <c r="G53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E54" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId86" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
+    <hyperlink ref="E15" r:id="rId292" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
@@ -3039,8 +3376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DBC0D3-CECE-4FBE-AFB4-B36031420D19}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3231,7 +3568,7 @@
         <v>88</v>
       </c>
       <c r="G9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3261,19 +3598,19 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F11" t="s">
         <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3284,7 +3621,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>81</v>
@@ -3296,7 +3633,7 @@
         <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3307,7 +3644,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -3319,7 +3656,7 @@
         <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3330,19 +3667,19 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F14" t="s">
         <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3353,19 +3690,19 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F15" t="s">
         <v>88</v>
       </c>
       <c r="G15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3376,7 +3713,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
@@ -3386,7 +3723,7 @@
         <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -3447,7 +3784,7 @@
         <v>88</v>
       </c>
       <c r="G19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -3563,19 +3900,19 @@
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="F25" t="s">
         <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -3589,14 +3926,14 @@
         <v>18</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" t="s">
         <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -3613,13 +3950,13 @@
         <v>6</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F27" t="s">
         <v>88</v>
       </c>
       <c r="G27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3720,7 +4057,7 @@
         <v>88</v>
       </c>
       <c r="G32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TA-01/ Modified script of Admin Scenario
</commit_message>
<xml_diff>
--- a/tests/testscenarios.xlsx
+++ b/tests/testscenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="12240" windowHeight="7830" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="233">
   <si>
     <t>Test Step</t>
   </si>
@@ -675,7 +675,7 @@
     <t>clicked on CREATEUSER_SUBMIT</t>
   </si>
   <si>
-    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                 Error: The username is already in use.</t>
+    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                                     </t>
   </si>
   <si>
     <t>clicked on CREATEUSERMENU_CLOSEBUTTON</t>
@@ -712,6 +712,12 @@
   </si>
   <si>
     <t>clicked on DELETEAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                 User AutomationUser created successfully.                    </t>
+  </si>
+  <si>
+    <t>Accepted  </t>
   </si>
 </sst>
 </file>
@@ -2040,7 +2046,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E22" r:id="rId292" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
+    <hyperlink ref="E22" r:id="rId422" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -2232,10 +2238,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB88CC8-F150-4CAF-B716-3BC4266F1F49}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G34" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2247,7 +2253,7 @@
     <col min="5" max="5" width="16.85546875" hidden="false" bestFit="false" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2264,7 +2270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2283,7 +2289,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2306,7 +2312,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2329,7 +2335,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2350,7 +2356,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -2369,7 +2375,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -2390,7 +2396,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2409,7 +2415,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -2430,7 +2436,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -2449,7 +2455,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -2470,7 +2476,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -2489,7 +2495,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -2512,7 +2518,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -2535,7 +2541,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -2558,7 +2564,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -2581,7 +2587,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
@@ -2604,7 +2610,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
@@ -2625,7 +2631,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -2645,10 +2651,10 @@
         <v>88</v>
       </c>
       <c r="G19" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
@@ -2669,7 +2675,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>83</v>
       </c>
@@ -2690,7 +2696,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>84</v>
       </c>
@@ -2709,7 +2715,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>85</v>
       </c>
@@ -2730,7 +2736,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>86</v>
       </c>
@@ -2749,7 +2755,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>163</v>
       </c>
@@ -2772,7 +2778,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>164</v>
       </c>
@@ -2795,7 +2801,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>165</v>
       </c>
@@ -2816,7 +2822,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>166</v>
       </c>
@@ -2835,7 +2841,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>167</v>
       </c>
@@ -2856,7 +2862,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>169</v>
       </c>
@@ -2875,7 +2881,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>172</v>
       </c>
@@ -2896,7 +2902,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>173</v>
       </c>
@@ -2915,7 +2921,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>174</v>
       </c>
@@ -2938,7 +2944,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>175</v>
       </c>
@@ -2961,7 +2967,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>176</v>
       </c>
@@ -2982,7 +2988,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>177</v>
       </c>
@@ -3001,7 +3007,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>178</v>
       </c>
@@ -3022,7 +3028,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>179</v>
       </c>
@@ -3041,7 +3047,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>180</v>
       </c>
@@ -3062,7 +3068,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>181</v>
       </c>
@@ -3081,7 +3087,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>182</v>
       </c>
@@ -3104,7 +3110,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>183</v>
       </c>
@@ -3125,7 +3131,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>184</v>
       </c>
@@ -3148,7 +3154,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>190</v>
       </c>
@@ -3169,7 +3175,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>192</v>
       </c>
@@ -3188,7 +3194,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>193</v>
       </c>
@@ -3211,7 +3217,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>196</v>
       </c>
@@ -3232,7 +3238,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>198</v>
       </c>
@@ -3253,7 +3259,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>200</v>
       </c>
@@ -3272,7 +3278,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>201</v>
       </c>
@@ -3293,7 +3299,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>203</v>
       </c>
@@ -3312,7 +3318,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>204</v>
       </c>
@@ -3333,7 +3339,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>207</v>
       </c>
@@ -3352,7 +3358,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>208</v>
       </c>
@@ -3362,10 +3368,16 @@
         <v>206</v>
       </c>
       <c r="E54" s="1"/>
+      <c r="F54" t="s">
+        <v>88</v>
+      </c>
+      <c r="G54" t="s">
+        <v>232</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId292" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
+    <hyperlink ref="E15" r:id="rId422" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>

</xml_diff>

<commit_message>
TA-01/ Admin Scenario modified with verification of deleted user
</commit_message>
<xml_diff>
--- a/tests/testscenarios.xlsx
+++ b/tests/testscenarios.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="232">
   <si>
     <t>Test Step</t>
   </si>
@@ -675,7 +675,7 @@
     <t>clicked on CREATEUSER_SUBMIT</t>
   </si>
   <si>
-    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                                     </t>
+    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                 User AutomationUser created successfully.                    </t>
   </si>
   <si>
     <t>clicked on CREATEUSERMENU_CLOSEBUTTON</t>
@@ -693,7 +693,7 @@
     <t>clicked on FILTER_BUTTON</t>
   </si>
   <si>
-    <t>Found FILTER_TABLE</t>
+    <t>Element FILTER_TABLE not found</t>
   </si>
   <si>
     <t>clicked on EDITAUTOMATIONUSER</t>
@@ -712,9 +712,6 @@
   </si>
   <si>
     <t>clicked on DELETEAUTOMATIONUSER</t>
-  </si>
-  <si>
-    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                 User AutomationUser created successfully.                    </t>
   </si>
   <si>
     <t>Accepted  </t>
@@ -2046,7 +2043,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E22" r:id="rId422" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
+    <hyperlink ref="E22" r:id="rId124" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -2238,10 +2235,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB88CC8-F150-4CAF-B716-3BC4266F1F49}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G34" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2651,7 +2648,7 @@
         <v>88</v>
       </c>
       <c r="G19" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3148,7 +3145,7 @@
         <v>151</v>
       </c>
       <c r="F43" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="G43" t="s">
         <v>224</v>
@@ -3372,12 +3369,182 @@
         <v>88</v>
       </c>
       <c r="G54" t="s">
-        <v>232</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" t="s">
+        <v>88</v>
+      </c>
+      <c r="G55" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" t="s">
+        <v>88</v>
+      </c>
+      <c r="G56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" t="s">
+        <v>88</v>
+      </c>
+      <c r="G57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" t="s">
+        <v>88</v>
+      </c>
+      <c r="G58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F59" t="s">
+        <v>88</v>
+      </c>
+      <c r="G59" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F60" t="s">
+        <v>88</v>
+      </c>
+      <c r="G60" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" t="s">
+        <v>88</v>
+      </c>
+      <c r="G61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F62" t="s">
+        <v>88</v>
+      </c>
+      <c r="G62" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId422" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
+    <hyperlink ref="E15" r:id="rId124" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
@@ -3388,8 +3555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DBC0D3-CECE-4FBE-AFB4-B36031420D19}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TA-02/Change company Scenario added
</commit_message>
<xml_diff>
--- a/tests/testscenarios.xlsx
+++ b/tests/testscenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="240">
   <si>
     <t>Test Step</t>
   </si>
@@ -378,9 +378,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t xml:space="preserve">id </t>
-  </si>
-  <si>
     <t>CHANGECOMPANY_LINK</t>
   </si>
   <si>
@@ -582,139 +579,166 @@
     <t>FILTER_TABLE</t>
   </si>
   <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>TS52</t>
+  </si>
+  <si>
+    <t>EDITAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>TS53</t>
+  </si>
+  <si>
+    <t>TS54</t>
+  </si>
+  <si>
+    <t>EDITUSER_TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit User </t>
+  </si>
+  <si>
+    <t>TS55</t>
+  </si>
+  <si>
+    <t>ADMINROLE_CHECKBOX</t>
+  </si>
+  <si>
+    <t>TS56</t>
+  </si>
+  <si>
+    <t>UPDATEBUTTON_EDITSCREEN</t>
+  </si>
+  <si>
+    <t>TS57</t>
+  </si>
+  <si>
+    <t>TS58</t>
+  </si>
+  <si>
+    <t>EDITSCREEN_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>TS59</t>
+  </si>
+  <si>
+    <t>TS60</t>
+  </si>
+  <si>
+    <t>DELETEAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>accept alert</t>
+  </si>
+  <si>
+    <t>TS61</t>
+  </si>
+  <si>
+    <t>TS62</t>
+  </si>
+  <si>
+    <t>clicked on ADMIN_LINK</t>
+  </si>
+  <si>
+    <t>clicked on CREATE_NEWUSER</t>
+  </si>
+  <si>
+    <t>Waiting for 1000 millisecond  text box to be present</t>
+  </si>
+  <si>
+    <t>Element present : CREATEUSER_TITLE</t>
+  </si>
+  <si>
+    <t>Typed AutomationUser into CREATEUSER_USERNAME text box</t>
+  </si>
+  <si>
+    <t>Typed nandini.rajaram@interfacesys.com into CREATEUSER_EMAIL text box</t>
+  </si>
+  <si>
+    <t>Typed Auto123 into CREATEUSER_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Typed Auto123 into CREATEUSER_CONFIRMPASSWORD text box</t>
+  </si>
+  <si>
+    <t>clicked on CREATEUSER_SUBMIT</t>
+  </si>
+  <si>
+    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                 User AutomationUser created successfully.</t>
+  </si>
+  <si>
+    <t>clicked on CREATEUSERMENU_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>Typed AutomationUser into USERNAME_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t>Typed Auto123 into PASSWORD_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t>Typed AutomationUser into FILTER_USERNAME text box</t>
+  </si>
+  <si>
+    <t>clicked on FILTER_BUTTON</t>
+  </si>
+  <si>
+    <t>Element FILTER_TABLE not found</t>
+  </si>
+  <si>
+    <t>clicked on EDITAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>Element present : Edit User</t>
+  </si>
+  <si>
+    <t>clicked on ADMINROLE_CHECKBOX</t>
+  </si>
+  <si>
+    <t>clicked on UPDATEBUTTON_EDITSCREEN</t>
+  </si>
+  <si>
+    <t>clicked on EDITSCREEN_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>clicked on DELETEAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>25000</t>
+  </si>
+  <si>
+    <t>COMPANY_DROPDOWN</t>
+  </si>
+  <si>
+    <t>DOLLAR EXPRESS</t>
+  </si>
+  <si>
+    <t>ChangeCompany_button</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>Waiting for 25000 millisecond  text box to be present</t>
+  </si>
+  <si>
     <t>clicked on CHANGECOMPANY_LINK</t>
   </si>
   <si>
-    <t>5000</t>
-  </si>
-  <si>
     <t>Waiting for 5000 millisecond  text box to be present</t>
   </si>
   <si>
-    <t>TS52</t>
-  </si>
-  <si>
-    <t>EDITAUTOMATIONUSER</t>
-  </si>
-  <si>
-    <t>TS53</t>
-  </si>
-  <si>
-    <t>TS54</t>
-  </si>
-  <si>
-    <t>EDITUSER_TITLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edit User </t>
-  </si>
-  <si>
-    <t>TS55</t>
-  </si>
-  <si>
-    <t>ADMINROLE_CHECKBOX</t>
-  </si>
-  <si>
-    <t>TS56</t>
-  </si>
-  <si>
-    <t>UPDATEBUTTON_EDITSCREEN</t>
-  </si>
-  <si>
-    <t>TS57</t>
-  </si>
-  <si>
-    <t>TS58</t>
-  </si>
-  <si>
-    <t>EDITSCREEN_CLOSEBUTTON</t>
-  </si>
-  <si>
-    <t>TS59</t>
-  </si>
-  <si>
-    <t>TS60</t>
-  </si>
-  <si>
-    <t>DELETEAUTOMATIONUSER</t>
-  </si>
-  <si>
-    <t>accept alert</t>
-  </si>
-  <si>
-    <t>TS61</t>
-  </si>
-  <si>
-    <t>TS62</t>
-  </si>
-  <si>
-    <t>clicked on ADMIN_LINK</t>
-  </si>
-  <si>
-    <t>clicked on CREATE_NEWUSER</t>
-  </si>
-  <si>
-    <t>Waiting for 1000 millisecond  text box to be present</t>
-  </si>
-  <si>
-    <t>Element present : CREATEUSER_TITLE</t>
-  </si>
-  <si>
-    <t>Typed AutomationUser into CREATEUSER_USERNAME text box</t>
-  </si>
-  <si>
-    <t>Typed nandini.rajaram@interfacesys.com into CREATEUSER_EMAIL text box</t>
-  </si>
-  <si>
-    <t>Typed Auto123 into CREATEUSER_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Typed Auto123 into CREATEUSER_CONFIRMPASSWORD text box</t>
-  </si>
-  <si>
-    <t>clicked on CREATEUSER_SUBMIT</t>
-  </si>
-  <si>
-    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                 User AutomationUser created successfully.                    </t>
-  </si>
-  <si>
-    <t>clicked on CREATEUSERMENU_CLOSEBUTTON</t>
-  </si>
-  <si>
-    <t>Typed AutomationUser into USERNAME_TEXTBOX text box</t>
-  </si>
-  <si>
-    <t>Typed Auto123 into PASSWORD_TEXTBOX text box</t>
-  </si>
-  <si>
-    <t>Typed AutomationUser into FILTER_USERNAME text box</t>
-  </si>
-  <si>
-    <t>clicked on FILTER_BUTTON</t>
-  </si>
-  <si>
-    <t>Element FILTER_TABLE not found</t>
-  </si>
-  <si>
-    <t>clicked on EDITAUTOMATIONUSER</t>
-  </si>
-  <si>
-    <t>Element present : Edit User</t>
-  </si>
-  <si>
-    <t>clicked on ADMINROLE_CHECKBOX</t>
-  </si>
-  <si>
-    <t>clicked on UPDATEBUTTON_EDITSCREEN</t>
-  </si>
-  <si>
-    <t>clicked on EDITSCREEN_CLOSEBUTTON</t>
-  </si>
-  <si>
-    <t>clicked on DELETEAUTOMATIONUSER</t>
-  </si>
-  <si>
-    <t>Accepted  </t>
+    <t>Selected the field  COMPANY_DROPDOWN</t>
+  </si>
+  <si>
+    <t>clicked on ChangeCompany_button</t>
+  </si>
+  <si>
+    <t>Waiting for 10000 millisecond  text box to be present</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1132,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1170,7 @@
         <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1159,10 +1183,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2043,7 +2067,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E22" r:id="rId124" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
+    <hyperlink ref="E22" r:id="rId62" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -2052,19 +2076,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C24C14-A866-4140-B688-97F68D23BE6D}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="27.5703125" hidden="false" bestFit="false" style="0"/>
     <col min="4" max="4" width="20.140625" hidden="false" bestFit="false" style="0"/>
+    <col min="5" max="5" width="15.85546875" hidden="false" bestFit="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2081,7 +2106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2100,7 +2125,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2120,10 +2145,10 @@
         <v>88</v>
       </c>
       <c r="G3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2146,7 +2171,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -2167,7 +2192,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -2177,24 +2202,24 @@
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>188</v>
+        <v>229</v>
       </c>
       <c r="F6" t="s">
         <v>88</v>
       </c>
       <c r="G6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C7" t="s">
-        <v>120</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
@@ -2204,10 +2229,10 @@
         <v>88</v>
       </c>
       <c r="G7" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -2217,15 +2242,176 @@
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
+        <v>186</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" t="s">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2235,10 +2421,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB88CC8-F150-4CAF-B716-3BC4266F1F49}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,7 +2436,7 @@
     <col min="5" max="5" width="16.85546875" hidden="false" bestFit="false" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2267,7 +2453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2286,7 +2472,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2306,10 +2492,10 @@
         <v>88</v>
       </c>
       <c r="G3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2332,7 +2518,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2353,7 +2539,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -2372,7 +2558,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -2393,7 +2579,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2412,7 +2598,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -2420,7 +2606,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
@@ -2430,10 +2616,10 @@
         <v>88</v>
       </c>
       <c r="G9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -2452,7 +2638,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -2460,7 +2646,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
@@ -2470,10 +2656,10 @@
         <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -2483,16 +2669,16 @@
         <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F12" t="s">
         <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -2500,22 +2686,22 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F13" t="s">
         <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -2523,22 +2709,22 @@
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F14" t="s">
         <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -2546,22 +2732,22 @@
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F15" t="s">
         <v>88</v>
       </c>
       <c r="G15" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -2569,22 +2755,22 @@
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F16" t="s">
         <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
@@ -2592,22 +2778,22 @@
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F17" t="s">
         <v>88</v>
       </c>
       <c r="G17" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
@@ -2615,7 +2801,7 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
@@ -2625,10 +2811,10 @@
         <v>88</v>
       </c>
       <c r="G18" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -2636,22 +2822,22 @@
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="F19" t="s">
         <v>88</v>
       </c>
       <c r="G19" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
@@ -2659,7 +2845,7 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>10</v>
@@ -2669,10 +2855,10 @@
         <v>88</v>
       </c>
       <c r="G20" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>83</v>
       </c>
@@ -2693,7 +2879,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>84</v>
       </c>
@@ -2712,7 +2898,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>85</v>
       </c>
@@ -2730,10 +2916,10 @@
         <v>88</v>
       </c>
       <c r="G23" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>86</v>
       </c>
@@ -2752,9 +2938,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -2766,18 +2952,18 @@
         <v>6</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F25" t="s">
         <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>9</v>
@@ -2789,18 +2975,18 @@
         <v>6</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F26" t="s">
         <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>9</v>
@@ -2819,9 +3005,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2838,9 +3024,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>11</v>
@@ -2859,9 +3045,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2878,9 +3064,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
@@ -2896,12 +3082,12 @@
         <v>88</v>
       </c>
       <c r="G31" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2918,9 +3104,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>9</v>
@@ -2938,12 +3124,12 @@
         <v>88</v>
       </c>
       <c r="G33" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>9</v>
@@ -2964,9 +3150,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>9</v>
@@ -2985,9 +3171,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3004,9 +3190,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>11</v>
@@ -3025,9 +3211,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3044,15 +3230,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>10</v>
@@ -3062,12 +3248,12 @@
         <v>88</v>
       </c>
       <c r="G39" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3084,38 +3270,38 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F41" t="s">
         <v>88</v>
       </c>
       <c r="G41" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>10</v>
@@ -3125,41 +3311,41 @@
         <v>88</v>
       </c>
       <c r="G42" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F43" t="s">
         <v>100</v>
       </c>
       <c r="G43" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>10</v>
@@ -3169,12 +3355,12 @@
         <v>88</v>
       </c>
       <c r="G44" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3191,38 +3377,38 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F46" t="s">
         <v>88</v>
       </c>
       <c r="G46" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>10</v>
@@ -3232,18 +3418,18 @@
         <v>88</v>
       </c>
       <c r="G47" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>10</v>
@@ -3253,12 +3439,12 @@
         <v>88</v>
       </c>
       <c r="G48" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3275,15 +3461,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>10</v>
@@ -3293,12 +3479,12 @@
         <v>88</v>
       </c>
       <c r="G50" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3315,15 +3501,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>10</v>
@@ -3333,12 +3519,12 @@
         <v>88</v>
       </c>
       <c r="G52" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3355,24 +3541,24 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" t="s">
         <v>88</v>
       </c>
       <c r="G54" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>83</v>
       </c>
@@ -3393,7 +3579,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>84</v>
       </c>
@@ -3412,7 +3598,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>85</v>
       </c>
@@ -3430,10 +3616,10 @@
         <v>88</v>
       </c>
       <c r="G57" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>86</v>
       </c>
@@ -3452,9 +3638,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>9</v>
@@ -3466,18 +3652,18 @@
         <v>6</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F59" t="s">
         <v>88</v>
       </c>
       <c r="G59" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>9</v>
@@ -3489,18 +3675,18 @@
         <v>6</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F60" t="s">
         <v>88</v>
       </c>
       <c r="G60" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>9</v>
@@ -3519,7 +3705,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>57</v>
       </c>
@@ -3527,24 +3713,24 @@
         <v>11</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="F62" t="s">
         <v>88</v>
       </c>
       <c r="G62" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId124" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
+    <hyperlink ref="E15" r:id="rId62" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
@@ -3623,7 +3809,7 @@
         <v>88</v>
       </c>
       <c r="G3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3747,7 +3933,7 @@
         <v>88</v>
       </c>
       <c r="G9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3777,19 +3963,19 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F11" t="s">
         <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3800,7 +3986,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>81</v>
@@ -3812,7 +3998,7 @@
         <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3823,7 +4009,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -3835,7 +4021,7 @@
         <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3846,19 +4032,19 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F14" t="s">
         <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3869,19 +4055,19 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F15" t="s">
         <v>88</v>
       </c>
       <c r="G15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3892,7 +4078,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
@@ -3902,7 +4088,7 @@
         <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -3963,7 +4149,7 @@
         <v>88</v>
       </c>
       <c r="G19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -4024,7 +4210,7 @@
         <v>88</v>
       </c>
       <c r="G22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -4079,19 +4265,19 @@
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="F25" t="s">
         <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -4105,14 +4291,14 @@
         <v>18</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" t="s">
         <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -4129,13 +4315,13 @@
         <v>6</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F27" t="s">
         <v>88</v>
       </c>
       <c r="G27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4236,7 +4422,7 @@
         <v>88</v>
       </c>
       <c r="G32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TA-04 / Search Files commit
</commit_message>
<xml_diff>
--- a/tests/testscenarios.xlsx
+++ b/tests/testscenarios.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -13,13 +13,16 @@
     <sheet name="ChangeCompany" sheetId="8" r:id="rId4"/>
     <sheet name="Administration" sheetId="10" r:id="rId5"/>
     <sheet name="Settings" sheetId="9" r:id="rId6"/>
+    <sheet name="Search" sheetId="11" r:id="rId7"/>
+    <sheet name="LogoVerification " sheetId="12" r:id="rId8"/>
+    <sheet name="SiteOverview" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="259">
   <si>
     <t>Test Step</t>
   </si>
@@ -375,390 +378,434 @@
     <t>Vishak.Nair</t>
   </si>
   <si>
+    <t>CHANGECOMPANY_LINK</t>
+  </si>
+  <si>
+    <t>Typed Vishak.Nair into USERNAME_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Settings </t>
+  </si>
+  <si>
+    <t>USER_SETTINGS</t>
+  </si>
+  <si>
+    <t>verifyElement</t>
+  </si>
+  <si>
+    <t>OLD_PASSWORD</t>
+  </si>
+  <si>
+    <t>NEW_PASSWORD</t>
+  </si>
+  <si>
+    <t>CONFIRM_PASSWORD</t>
+  </si>
+  <si>
+    <t>UPDATE_BUTTON</t>
+  </si>
+  <si>
+    <t>Interface2</t>
+  </si>
+  <si>
+    <t>USER_NAME_SETTINGS</t>
+  </si>
+  <si>
+    <t>LOGIN_ERRORMSG</t>
+  </si>
+  <si>
+    <t>Login Error: The username/password you provided were incorrect.</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>ADMIN_LINK</t>
+  </si>
+  <si>
+    <t>getTextContent</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>clicked on SETTINGS_LINK</t>
+  </si>
+  <si>
+    <t>Element present : USER_SETTINGS</t>
+  </si>
+  <si>
+    <t>Element present : vishak.nair</t>
+  </si>
+  <si>
+    <t>Typed Interface1 into OLD_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Typed Interface2 into NEW_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Typed Interface2 into CONFIRM_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>clicked on UPDATE_BUTTON</t>
+  </si>
+  <si>
+    <t>clicked on LOGOUT_LINK</t>
+  </si>
+  <si>
+    <t>clear the field  PASSWORD_TEXTBOX</t>
+  </si>
+  <si>
+    <t>Typed Interface2 into PASSWORD_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t>Element present : Login Error: The username/password you provided were incorrect.</t>
+  </si>
+  <si>
+    <t>CREATE_NEWUSER</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>CREATEUSER_USERNAME</t>
+  </si>
+  <si>
+    <t>AutomationUser</t>
+  </si>
+  <si>
+    <t>Create User</t>
+  </si>
+  <si>
+    <t>CREATEUSER_TITLE</t>
+  </si>
+  <si>
+    <t>CREATEUSER_EMAIL</t>
+  </si>
+  <si>
+    <t>CREATEUSER_PASSWORD</t>
+  </si>
+  <si>
+    <t>CREATEUSER_CONFIRMPASSWORD</t>
+  </si>
+  <si>
+    <t>nandini.rajaram@interfacesys.com</t>
+  </si>
+  <si>
+    <t>Auto123</t>
+  </si>
+  <si>
+    <t>CREATEUSER_SUBMIT</t>
+  </si>
+  <si>
+    <t>USERCREATION_SUCCESSMESSAGE</t>
+  </si>
+  <si>
+    <t>User Automation User created successfully.</t>
+  </si>
+  <si>
+    <t>CREATEUSERMENU_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>TS33</t>
+  </si>
+  <si>
+    <t>TS34</t>
+  </si>
+  <si>
+    <t>TS35</t>
+  </si>
+  <si>
+    <t>TS36</t>
+  </si>
+  <si>
+    <t>TS37</t>
+  </si>
+  <si>
+    <t>FILTER_USERNAME</t>
+  </si>
+  <si>
+    <t>TS38</t>
+  </si>
+  <si>
+    <t>FILTER_BUTTON</t>
+  </si>
+  <si>
+    <t>partialLinkText</t>
+  </si>
+  <si>
+    <t>TS39</t>
+  </si>
+  <si>
+    <t>TS40</t>
+  </si>
+  <si>
+    <t>TS41</t>
+  </si>
+  <si>
+    <t>TS42</t>
+  </si>
+  <si>
+    <t>TS43</t>
+  </si>
+  <si>
+    <t>TS44</t>
+  </si>
+  <si>
+    <t>TS45</t>
+  </si>
+  <si>
+    <t>TS46</t>
+  </si>
+  <si>
+    <t>TS47</t>
+  </si>
+  <si>
+    <t>TS48</t>
+  </si>
+  <si>
+    <t>TS49</t>
+  </si>
+  <si>
+    <t>TS50</t>
+  </si>
+  <si>
+    <t>TS51</t>
+  </si>
+  <si>
+    <t>searchElement</t>
+  </si>
+  <si>
+    <t>FILTER_TABLE</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>TS52</t>
+  </si>
+  <si>
+    <t>EDITAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>TS53</t>
+  </si>
+  <si>
+    <t>TS54</t>
+  </si>
+  <si>
+    <t>EDITUSER_TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit User </t>
+  </si>
+  <si>
+    <t>TS55</t>
+  </si>
+  <si>
+    <t>ADMINROLE_CHECKBOX</t>
+  </si>
+  <si>
+    <t>TS56</t>
+  </si>
+  <si>
+    <t>UPDATEBUTTON_EDITSCREEN</t>
+  </si>
+  <si>
+    <t>TS57</t>
+  </si>
+  <si>
+    <t>TS58</t>
+  </si>
+  <si>
+    <t>EDITSCREEN_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>TS59</t>
+  </si>
+  <si>
+    <t>TS60</t>
+  </si>
+  <si>
+    <t>DELETEAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>accept alert</t>
+  </si>
+  <si>
+    <t>TS61</t>
+  </si>
+  <si>
+    <t>TS62</t>
+  </si>
+  <si>
+    <t>clicked on ADMIN_LINK</t>
+  </si>
+  <si>
+    <t>clicked on CREATE_NEWUSER</t>
+  </si>
+  <si>
+    <t>Waiting for 1000 millisecond  text box to be present</t>
+  </si>
+  <si>
+    <t>Element present : CREATEUSER_TITLE</t>
+  </si>
+  <si>
+    <t>Typed AutomationUser into CREATEUSER_USERNAME text box</t>
+  </si>
+  <si>
+    <t>Typed nandini.rajaram@interfacesys.com into CREATEUSER_EMAIL text box</t>
+  </si>
+  <si>
+    <t>Typed Auto123 into CREATEUSER_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Typed Auto123 into CREATEUSER_CONFIRMPASSWORD text box</t>
+  </si>
+  <si>
+    <t>clicked on CREATEUSER_SUBMIT</t>
+  </si>
+  <si>
+    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                 User AutomationUser created successfully.</t>
+  </si>
+  <si>
+    <t>clicked on CREATEUSERMENU_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>Typed AutomationUser into USERNAME_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t>Typed Auto123 into PASSWORD_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t>Typed AutomationUser into FILTER_USERNAME text box</t>
+  </si>
+  <si>
+    <t>clicked on FILTER_BUTTON</t>
+  </si>
+  <si>
+    <t>Element FILTER_TABLE not found</t>
+  </si>
+  <si>
+    <t>clicked on EDITAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>Element present : Edit User</t>
+  </si>
+  <si>
+    <t>clicked on ADMINROLE_CHECKBOX</t>
+  </si>
+  <si>
+    <t>clicked on UPDATEBUTTON_EDITSCREEN</t>
+  </si>
+  <si>
+    <t>clicked on EDITSCREEN_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>clicked on DELETEAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>25000</t>
+  </si>
+  <si>
+    <t>COMPANY_DROPDOWN</t>
+  </si>
+  <si>
+    <t>DOLLAR EXPRESS</t>
+  </si>
+  <si>
+    <t>ChangeCompany_button</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>Waiting for 25000 millisecond  text box to be present</t>
+  </si>
+  <si>
+    <t>clicked on CHANGECOMPANY_LINK</t>
+  </si>
+  <si>
+    <t>Waiting for 5000 millisecond  text box to be present</t>
+  </si>
+  <si>
+    <t>clicked on ChangeCompany_button</t>
+  </si>
+  <si>
+    <t>Waiting for 10000 millisecond  text box to be present</t>
+  </si>
+  <si>
+    <t>Element COMPANY_DROPDOWN not found</t>
+  </si>
+  <si>
+    <t>Typed Interface2 into OLD_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Typed Interface1 into NEW_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Typed Interface1 into CONFIRM_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>SEARCH_FIELD</t>
+  </si>
+  <si>
+    <t>SEARCHRESULT</t>
+  </si>
+  <si>
+    <t>1442</t>
+  </si>
+  <si>
+    <t>callSearchObject</t>
+  </si>
+  <si>
+    <t>Typed 1442 into SEARCH_FIELD text box</t>
+  </si>
+  <si>
+    <t>clicked on SEARCHRESULT</t>
+  </si>
+  <si>
+    <t>Verified the address</t>
+  </si>
+  <si>
+    <t>ONEVIEWLOGO</t>
+  </si>
+  <si>
+    <t>LogoVerification</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
-    <t>CHANGECOMPANY_LINK</t>
-  </si>
-  <si>
-    <t>Typed Vishak.Nair into USERNAME_TEXTBOX text box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Settings </t>
-  </si>
-  <si>
-    <t>USER_SETTINGS</t>
-  </si>
-  <si>
-    <t>verifyElement</t>
-  </si>
-  <si>
-    <t>OLD_PASSWORD</t>
-  </si>
-  <si>
-    <t>NEW_PASSWORD</t>
-  </si>
-  <si>
-    <t>CONFIRM_PASSWORD</t>
-  </si>
-  <si>
-    <t>UPDATE_BUTTON</t>
-  </si>
-  <si>
-    <t>Interface2</t>
-  </si>
-  <si>
-    <t>USER_NAME_SETTINGS</t>
-  </si>
-  <si>
-    <t>LOGIN_ERRORMSG</t>
-  </si>
-  <si>
-    <t>Login Error: The username/password you provided were incorrect.</t>
-  </si>
-  <si>
-    <t>clear</t>
-  </si>
-  <si>
-    <t>ADMIN_LINK</t>
-  </si>
-  <si>
-    <t>getTextContent</t>
-  </si>
-  <si>
-    <t>Administration</t>
-  </si>
-  <si>
-    <t>clicked on SETTINGS_LINK</t>
-  </si>
-  <si>
-    <t>Element present : USER_SETTINGS</t>
-  </si>
-  <si>
-    <t>Element present : vishak.nair</t>
-  </si>
-  <si>
-    <t>Typed Interface1 into OLD_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Typed Interface2 into NEW_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Typed Interface2 into CONFIRM_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>clicked on UPDATE_BUTTON</t>
-  </si>
-  <si>
-    <t>clicked on LOGOUT_LINK</t>
-  </si>
-  <si>
-    <t>clear the field  PASSWORD_TEXTBOX</t>
-  </si>
-  <si>
-    <t>Typed Interface2 into PASSWORD_TEXTBOX text box</t>
-  </si>
-  <si>
-    <t>Element present : Login Error: The username/password you provided were incorrect.</t>
-  </si>
-  <si>
-    <t>CREATE_NEWUSER</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>CREATEUSER_USERNAME</t>
-  </si>
-  <si>
-    <t>AutomationUser</t>
-  </si>
-  <si>
-    <t>Create User</t>
-  </si>
-  <si>
-    <t>CREATEUSER_TITLE</t>
-  </si>
-  <si>
-    <t>CREATEUSER_EMAIL</t>
-  </si>
-  <si>
-    <t>CREATEUSER_PASSWORD</t>
-  </si>
-  <si>
-    <t>CREATEUSER_CONFIRMPASSWORD</t>
-  </si>
-  <si>
-    <t>nandini.rajaram@interfacesys.com</t>
-  </si>
-  <si>
-    <t>Auto123</t>
-  </si>
-  <si>
-    <t>CREATEUSER_SUBMIT</t>
-  </si>
-  <si>
-    <t>USERCREATION_SUCCESSMESSAGE</t>
-  </si>
-  <si>
-    <t>User Automation User created successfully.</t>
-  </si>
-  <si>
-    <t>CREATEUSERMENU_CLOSEBUTTON</t>
-  </si>
-  <si>
-    <t>TS33</t>
-  </si>
-  <si>
-    <t>TS34</t>
-  </si>
-  <si>
-    <t>TS35</t>
-  </si>
-  <si>
-    <t>TS36</t>
-  </si>
-  <si>
-    <t>TS37</t>
-  </si>
-  <si>
-    <t>FILTER_USERNAME</t>
-  </si>
-  <si>
-    <t>TS38</t>
-  </si>
-  <si>
-    <t>FILTER_BUTTON</t>
-  </si>
-  <si>
-    <t>partialLinkText</t>
-  </si>
-  <si>
-    <t>TS39</t>
-  </si>
-  <si>
-    <t>TS40</t>
-  </si>
-  <si>
-    <t>TS41</t>
-  </si>
-  <si>
-    <t>TS42</t>
-  </si>
-  <si>
-    <t>TS43</t>
-  </si>
-  <si>
-    <t>TS44</t>
-  </si>
-  <si>
-    <t>TS45</t>
-  </si>
-  <si>
-    <t>TS46</t>
-  </si>
-  <si>
-    <t>TS47</t>
-  </si>
-  <si>
-    <t>TS48</t>
-  </si>
-  <si>
-    <t>TS49</t>
-  </si>
-  <si>
-    <t>TS50</t>
-  </si>
-  <si>
-    <t>TS51</t>
-  </si>
-  <si>
-    <t>searchElement</t>
-  </si>
-  <si>
-    <t>FILTER_TABLE</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>TS52</t>
-  </si>
-  <si>
-    <t>EDITAUTOMATIONUSER</t>
-  </si>
-  <si>
-    <t>TS53</t>
-  </si>
-  <si>
-    <t>TS54</t>
-  </si>
-  <si>
-    <t>EDITUSER_TITLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edit User </t>
-  </si>
-  <si>
-    <t>TS55</t>
-  </si>
-  <si>
-    <t>ADMINROLE_CHECKBOX</t>
-  </si>
-  <si>
-    <t>TS56</t>
-  </si>
-  <si>
-    <t>UPDATEBUTTON_EDITSCREEN</t>
-  </si>
-  <si>
-    <t>TS57</t>
-  </si>
-  <si>
-    <t>TS58</t>
-  </si>
-  <si>
-    <t>EDITSCREEN_CLOSEBUTTON</t>
-  </si>
-  <si>
-    <t>TS59</t>
-  </si>
-  <si>
-    <t>TS60</t>
-  </si>
-  <si>
-    <t>DELETEAUTOMATIONUSER</t>
-  </si>
-  <si>
-    <t>accept alert</t>
-  </si>
-  <si>
-    <t>TS61</t>
-  </si>
-  <si>
-    <t>TS62</t>
-  </si>
-  <si>
-    <t>clicked on ADMIN_LINK</t>
-  </si>
-  <si>
-    <t>clicked on CREATE_NEWUSER</t>
-  </si>
-  <si>
-    <t>Waiting for 1000 millisecond  text box to be present</t>
-  </si>
-  <si>
-    <t>Element present : CREATEUSER_TITLE</t>
-  </si>
-  <si>
-    <t>Typed AutomationUser into CREATEUSER_USERNAME text box</t>
-  </si>
-  <si>
-    <t>Typed nandini.rajaram@interfacesys.com into CREATEUSER_EMAIL text box</t>
-  </si>
-  <si>
-    <t>Typed Auto123 into CREATEUSER_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Typed Auto123 into CREATEUSER_CONFIRMPASSWORD text box</t>
-  </si>
-  <si>
-    <t>clicked on CREATEUSER_SUBMIT</t>
-  </si>
-  <si>
-    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                 User AutomationUser created successfully.</t>
-  </si>
-  <si>
-    <t>clicked on CREATEUSERMENU_CLOSEBUTTON</t>
-  </si>
-  <si>
-    <t>Typed AutomationUser into USERNAME_TEXTBOX text box</t>
-  </si>
-  <si>
-    <t>Typed Auto123 into PASSWORD_TEXTBOX text box</t>
-  </si>
-  <si>
-    <t>Typed AutomationUser into FILTER_USERNAME text box</t>
-  </si>
-  <si>
-    <t>clicked on FILTER_BUTTON</t>
-  </si>
-  <si>
-    <t>Element FILTER_TABLE not found</t>
-  </si>
-  <si>
-    <t>clicked on EDITAUTOMATIONUSER</t>
-  </si>
-  <si>
-    <t>Element present : Edit User</t>
-  </si>
-  <si>
-    <t>clicked on ADMINROLE_CHECKBOX</t>
-  </si>
-  <si>
-    <t>clicked on UPDATEBUTTON_EDITSCREEN</t>
-  </si>
-  <si>
-    <t>clicked on EDITSCREEN_CLOSEBUTTON</t>
-  </si>
-  <si>
-    <t>clicked on DELETEAUTOMATIONUSER</t>
-  </si>
-  <si>
-    <t>Accepted</t>
-  </si>
-  <si>
-    <t>25000</t>
-  </si>
-  <si>
-    <t>COMPANY_DROPDOWN</t>
-  </si>
-  <si>
-    <t>DOLLAR EXPRESS</t>
-  </si>
-  <si>
-    <t>ChangeCompany_button</t>
-  </si>
-  <si>
-    <t>10000</t>
-  </si>
-  <si>
-    <t>Waiting for 25000 millisecond  text box to be present</t>
-  </si>
-  <si>
-    <t>clicked on CHANGECOMPANY_LINK</t>
-  </si>
-  <si>
-    <t>Waiting for 5000 millisecond  text box to be present</t>
-  </si>
-  <si>
-    <t>Selected the field  COMPANY_DROPDOWN</t>
-  </si>
-  <si>
-    <t>clicked on ChangeCompany_button</t>
-  </si>
-  <si>
-    <t>Waiting for 10000 millisecond  text box to be present</t>
-  </si>
-  <si>
-    <t>Element COMPANY_DROPDOWN not found</t>
-  </si>
-  <si>
-    <t>Typed Interface2 into OLD_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Typed Interface1 into NEW_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Typed Interface1 into CONFIRM_PASSWORD text box</t>
+    <t>http://oneviewdev.interfacesys.com/Main.aspx</t>
+  </si>
+  <si>
+    <t>verifyCurrentURL</t>
+  </si>
+  <si>
+    <t>clicked on ONEVIEWLOGO</t>
+  </si>
+  <si>
+    <t>Navigated to the Home page</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>SiteOverview</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1141,16 +1188,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" hidden="false" bestFit="false" style="0"/>
-    <col min="2" max="2" width="15.5703125" hidden="false" bestFit="true" style="0"/>
+    <col min="1" max="1" width="22.7109375"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1190,15 +1237,39 @@
         <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B9" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -1211,16 +1282,16 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E8"/>
+      <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" hidden="false" bestFit="true" style="0"/>
-    <col min="3" max="3" width="20.28515625" hidden="false" bestFit="true" style="0"/>
-    <col min="4" max="4" width="21.42578125" hidden="false" bestFit="false" style="0"/>
-    <col min="5" max="5" width="24.85546875" hidden="false" bestFit="true" style="0"/>
-    <col min="7" max="7" width="52.42578125" hidden="false" bestFit="false" style="0"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1"/>
+    <col min="4" max="4" width="21.42578125"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1"/>
+    <col min="7" max="7" width="52.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1388,8 +1459,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="29.7109375" hidden="false" bestFit="true" style="0"/>
-    <col min="5" max="5" width="20.28515625" hidden="false" bestFit="true" style="0"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2079,7 +2150,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E22" r:id="rId256" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
+    <hyperlink ref="E22" r:id="rId1" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -2096,9 +2167,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.5703125" hidden="false" bestFit="false" style="0"/>
-    <col min="4" max="4" width="20.140625" hidden="false" bestFit="false" style="0"/>
-    <col min="5" max="5" width="15.85546875" hidden="false" bestFit="true" style="0"/>
+    <col min="3" max="3" width="27.5703125"/>
+    <col min="4" max="4" width="20.140625"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2157,7 +2228,7 @@
         <v>88</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2214,13 +2285,13 @@
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F6" t="s">
         <v>88</v>
       </c>
       <c r="G6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2231,7 +2302,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
@@ -2241,7 +2312,7 @@
         <v>88</v>
       </c>
       <c r="G7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2254,13 +2325,13 @@
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F8" t="s">
         <v>88</v>
       </c>
       <c r="G8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2271,19 +2342,19 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F9" t="s">
         <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2296,13 +2367,13 @@
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F10" t="s">
         <v>88</v>
       </c>
       <c r="G10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2313,7 +2384,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
@@ -2323,7 +2394,7 @@
         <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2336,13 +2407,13 @@
         <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F12" t="s">
         <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2422,7 +2493,7 @@
         <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2441,11 +2512,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" hidden="false" bestFit="false" style="0"/>
-    <col min="2" max="2" width="25.140625" hidden="false" bestFit="false" style="0"/>
-    <col min="3" max="3" width="30.5703125" hidden="false" bestFit="false" style="0"/>
-    <col min="4" max="4" width="19.7109375" hidden="false" bestFit="false" style="0"/>
-    <col min="5" max="5" width="16.85546875" hidden="false" bestFit="false" style="0"/>
+    <col min="1" max="1" width="14.5703125"/>
+    <col min="2" max="2" width="25.140625"/>
+    <col min="3" max="3" width="30.5703125"/>
+    <col min="4" max="4" width="19.7109375"/>
+    <col min="5" max="5" width="16.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2504,7 +2575,7 @@
         <v>88</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2618,7 +2689,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
@@ -2628,7 +2699,7 @@
         <v>88</v>
       </c>
       <c r="G9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2658,7 +2729,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
@@ -2668,7 +2739,7 @@
         <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2681,13 +2752,13 @@
         <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F12" t="s">
         <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2698,19 +2769,19 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F13" t="s">
         <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2721,19 +2792,19 @@
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F14" t="s">
         <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2744,19 +2815,19 @@
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F15" t="s">
         <v>88</v>
       </c>
       <c r="G15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2767,19 +2838,19 @@
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F16" t="s">
         <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2790,19 +2861,19 @@
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F17" t="s">
         <v>88</v>
       </c>
       <c r="G17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2813,7 +2884,7 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
@@ -2823,7 +2894,7 @@
         <v>88</v>
       </c>
       <c r="G18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2834,19 +2905,19 @@
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="F19" t="s">
         <v>88</v>
       </c>
       <c r="G19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2857,7 +2928,7 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>10</v>
@@ -2867,7 +2938,7 @@
         <v>88</v>
       </c>
       <c r="G20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2928,7 +2999,7 @@
         <v>88</v>
       </c>
       <c r="G23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2952,7 +3023,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -2964,18 +3035,18 @@
         <v>6</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F25" t="s">
         <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>9</v>
@@ -2987,18 +3058,18 @@
         <v>6</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F26" t="s">
         <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>9</v>
@@ -3019,7 +3090,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3038,7 +3109,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>11</v>
@@ -3059,7 +3130,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3078,7 +3149,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
@@ -3094,12 +3165,12 @@
         <v>88</v>
       </c>
       <c r="G31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3118,7 +3189,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>9</v>
@@ -3136,12 +3207,12 @@
         <v>88</v>
       </c>
       <c r="G33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>9</v>
@@ -3164,7 +3235,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>9</v>
@@ -3185,7 +3256,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3204,7 +3275,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>11</v>
@@ -3225,7 +3296,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3244,13 +3315,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>10</v>
@@ -3260,12 +3331,12 @@
         <v>88</v>
       </c>
       <c r="G39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3284,36 +3355,36 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F41" t="s">
         <v>88</v>
       </c>
       <c r="G41" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>10</v>
@@ -3323,41 +3394,41 @@
         <v>88</v>
       </c>
       <c r="G42" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F43" t="s">
         <v>100</v>
       </c>
       <c r="G43" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>10</v>
@@ -3367,12 +3438,12 @@
         <v>88</v>
       </c>
       <c r="G44" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3391,36 +3462,36 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F46" t="s">
         <v>88</v>
       </c>
       <c r="G46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>10</v>
@@ -3430,18 +3501,18 @@
         <v>88</v>
       </c>
       <c r="G47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>10</v>
@@ -3451,12 +3522,12 @@
         <v>88</v>
       </c>
       <c r="G48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3475,13 +3546,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>10</v>
@@ -3491,12 +3562,12 @@
         <v>88</v>
       </c>
       <c r="G50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3515,13 +3586,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>10</v>
@@ -3531,12 +3602,12 @@
         <v>88</v>
       </c>
       <c r="G52" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3555,19 +3626,19 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" t="s">
         <v>88</v>
       </c>
       <c r="G54" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3628,7 +3699,7 @@
         <v>88</v>
       </c>
       <c r="G57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3652,7 +3723,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>9</v>
@@ -3664,18 +3735,18 @@
         <v>6</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F59" t="s">
         <v>88</v>
       </c>
       <c r="G59" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>9</v>
@@ -3687,18 +3758,18 @@
         <v>6</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F60" t="s">
         <v>88</v>
       </c>
       <c r="G60" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>9</v>
@@ -3725,24 +3796,24 @@
         <v>11</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="F62" t="s">
         <v>88</v>
       </c>
       <c r="G62" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId256" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
+    <hyperlink ref="E15" r:id="rId1" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
@@ -3759,10 +3830,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.42578125" hidden="false" bestFit="false" style="0"/>
-    <col min="4" max="4" width="18.7109375" hidden="false" bestFit="false" style="0"/>
-    <col min="5" max="5" width="73.28515625" hidden="false" bestFit="false" style="0"/>
-    <col min="7" max="7" width="48.28515625" hidden="false" bestFit="false" style="0"/>
+    <col min="3" max="3" width="21.42578125"/>
+    <col min="4" max="4" width="18.7109375"/>
+    <col min="5" max="5" width="73.28515625"/>
+    <col min="7" max="7" width="48.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3821,7 +3892,7 @@
         <v>88</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3945,7 +4016,7 @@
         <v>88</v>
       </c>
       <c r="G9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3975,19 +4046,19 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F11" t="s">
         <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3998,7 +4069,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>81</v>
@@ -4010,7 +4081,7 @@
         <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -4021,7 +4092,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -4033,7 +4104,7 @@
         <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4044,19 +4115,19 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F14" t="s">
         <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4067,19 +4138,19 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F15" t="s">
         <v>88</v>
       </c>
       <c r="G15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4090,7 +4161,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
@@ -4100,7 +4171,7 @@
         <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -4161,7 +4232,7 @@
         <v>88</v>
       </c>
       <c r="G19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -4222,7 +4293,7 @@
         <v>88</v>
       </c>
       <c r="G22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -4277,19 +4348,19 @@
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="F25" t="s">
         <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -4303,14 +4374,14 @@
         <v>18</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" t="s">
         <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -4327,13 +4398,13 @@
         <v>6</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F27" t="s">
         <v>88</v>
       </c>
       <c r="G27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4415,7 +4486,7 @@
         <v>88</v>
       </c>
       <c r="G31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -4437,7 +4508,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>86</v>
       </c>
@@ -4445,30 +4516,30 @@
         <v>11</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F33" t="s">
         <v>88</v>
       </c>
       <c r="G33" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>81</v>
@@ -4480,41 +4551,41 @@
         <v>88</v>
       </c>
       <c r="G34" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F35" t="s">
         <v>88</v>
       </c>
       <c r="G35" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>6</v>
@@ -4526,18 +4597,18 @@
         <v>88</v>
       </c>
       <c r="G36" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>6</v>
@@ -4549,18 +4620,18 @@
         <v>88</v>
       </c>
       <c r="G37" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>10</v>
@@ -4570,10 +4641,10 @@
         <v>88</v>
       </c>
       <c r="G38" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>49</v>
       </c>
@@ -4594,7 +4665,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>50</v>
       </c>
@@ -4613,7 +4684,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>51</v>
       </c>
@@ -4631,7 +4702,573 @@
         <v>88</v>
       </c>
       <c r="G41" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70AD2540-E285-4D45-A9DF-57EC1F4499A7}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125"/>
+    <col min="2" max="2" width="20.7109375"/>
+    <col min="3" max="3" width="24.140625"/>
+    <col min="4" max="4" width="19.140625"/>
+    <col min="5" max="5" width="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF64BA0D-1DB8-4A11-A7D2-47596EF1A22C}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625"/>
+    <col min="2" max="2" width="20.5703125"/>
+    <col min="3" max="3" width="19.7109375"/>
+    <col min="4" max="4" width="17.140625"/>
+    <col min="5" max="5" width="44.28515625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>250</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E13" t="s">
+        <v>253</v>
+      </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280F664A-D85A-4270-B867-390C9C41113A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TA-04/ Logo and Search
</commit_message>
<xml_diff>
--- a/tests/testscenarios.xlsx
+++ b/tests/testscenarios.xlsx
@@ -15,14 +15,13 @@
     <sheet name="Settings" sheetId="9" r:id="rId6"/>
     <sheet name="Search" sheetId="11" r:id="rId7"/>
     <sheet name="LogoVerification " sheetId="12" r:id="rId8"/>
-    <sheet name="SiteOverview" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="260">
   <si>
     <t>Test Step</t>
   </si>
@@ -795,17 +794,21 @@
     <t>Navigated to the Home page</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>SiteOverview</t>
+    <t>Element USERNAME_TEXTBOX not found</t>
+  </si>
+  <si>
+    <t>Element PASSWORD_TEXTBOX not found</t>
+  </si>
+  <si>
+    <t>Element SUBMIT_BUTTON not found</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1188,16 +1191,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C14" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1"/>
+    <col min="1" max="1" width="22.7109375" hidden="false" bestFit="false" style="0"/>
+    <col min="2" max="2" width="15.5703125" hidden="false" bestFit="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1253,7 +1256,7 @@
         <v>242</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1261,14 +1264,6 @@
         <v>251</v>
       </c>
       <c r="B8" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>258</v>
-      </c>
-      <c r="B9" t="s">
         <v>252</v>
       </c>
     </row>
@@ -1287,11 +1282,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" bestFit="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1"/>
-    <col min="4" max="4" width="21.42578125"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1"/>
-    <col min="7" max="7" width="52.42578125"/>
+    <col min="2" max="2" width="18.42578125" hidden="false" bestFit="true" style="0"/>
+    <col min="3" max="3" width="20.28515625" hidden="false" bestFit="true" style="0"/>
+    <col min="4" max="4" width="21.42578125" hidden="false" bestFit="false" style="0"/>
+    <col min="5" max="5" width="24.85546875" hidden="false" bestFit="true" style="0"/>
+    <col min="7" max="7" width="52.42578125" hidden="false" bestFit="false" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1459,8 +1454,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="29.7109375" bestFit="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1"/>
+    <col min="3" max="3" width="29.7109375" hidden="false" bestFit="true" style="0"/>
+    <col min="5" max="5" width="20.28515625" hidden="false" bestFit="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2150,7 +2145,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E22" r:id="rId1" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
+    <hyperlink ref="E22" r:id="rId30" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -2167,9 +2162,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.5703125"/>
-    <col min="4" max="4" width="20.140625"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1"/>
+    <col min="3" max="3" width="27.5703125" hidden="false" bestFit="false" style="0"/>
+    <col min="4" max="4" width="20.140625" hidden="false" bestFit="false" style="0"/>
+    <col min="5" max="5" width="15.85546875" hidden="false" bestFit="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2512,11 +2507,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125"/>
-    <col min="2" max="2" width="25.140625"/>
-    <col min="3" max="3" width="30.5703125"/>
-    <col min="4" max="4" width="19.7109375"/>
-    <col min="5" max="5" width="16.85546875"/>
+    <col min="1" max="1" width="14.5703125" hidden="false" bestFit="false" style="0"/>
+    <col min="2" max="2" width="25.140625" hidden="false" bestFit="false" style="0"/>
+    <col min="3" max="3" width="30.5703125" hidden="false" bestFit="false" style="0"/>
+    <col min="4" max="4" width="19.7109375" hidden="false" bestFit="false" style="0"/>
+    <col min="5" max="5" width="16.85546875" hidden="false" bestFit="false" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3813,7 +3808,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId1" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
+    <hyperlink ref="E15" r:id="rId30" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
@@ -3830,10 +3825,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.42578125"/>
-    <col min="4" max="4" width="18.7109375"/>
-    <col min="5" max="5" width="73.28515625"/>
-    <col min="7" max="7" width="48.28515625"/>
+    <col min="3" max="3" width="21.42578125" hidden="false" bestFit="false" style="0"/>
+    <col min="4" max="4" width="18.7109375" hidden="false" bestFit="false" style="0"/>
+    <col min="5" max="5" width="73.28515625" hidden="false" bestFit="false" style="0"/>
+    <col min="7" max="7" width="48.28515625" hidden="false" bestFit="false" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4720,11 +4715,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125"/>
-    <col min="2" max="2" width="20.7109375"/>
-    <col min="3" max="3" width="24.140625"/>
-    <col min="4" max="4" width="19.140625"/>
-    <col min="5" max="5" width="31"/>
+    <col min="1" max="1" width="13.42578125" hidden="false" bestFit="false" style="0"/>
+    <col min="2" max="2" width="20.7109375" hidden="false" bestFit="false" style="0"/>
+    <col min="3" max="3" width="24.140625" hidden="false" bestFit="false" style="0"/>
+    <col min="4" max="4" width="19.140625" hidden="false" bestFit="false" style="0"/>
+    <col min="5" max="5" width="31.0" hidden="false" bestFit="false" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4973,16 +4968,16 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection sqref="A1:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625"/>
-    <col min="2" max="2" width="20.5703125"/>
-    <col min="3" max="3" width="19.7109375"/>
-    <col min="4" max="4" width="17.140625"/>
-    <col min="5" max="5" width="44.28515625"/>
+    <col min="1" max="1" width="17.28515625" hidden="false" bestFit="false" style="0"/>
+    <col min="2" max="2" width="20.5703125" hidden="false" bestFit="false" style="0"/>
+    <col min="3" max="3" width="19.7109375" hidden="false" bestFit="false" style="0"/>
+    <col min="4" max="4" width="17.140625" hidden="false" bestFit="false" style="0"/>
+    <col min="5" max="5" width="44.28515625" hidden="false" bestFit="false" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5038,10 +5033,10 @@
         <v>117</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>119</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -5061,10 +5056,10 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -5082,10 +5077,10 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -5254,24 +5249,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280F664A-D85A-4270-B867-390C9C41113A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
TA-05 / SQL CHANGES
</commit_message>
<xml_diff>
--- a/tests/testscenarios.xlsx
+++ b/tests/testscenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="244">
   <si>
     <t>Test Step</t>
   </si>
@@ -263,9 +263,6 @@
     <t>CASESEARCH_TEXTBOX</t>
   </si>
   <si>
-    <t>Automationuser</t>
-  </si>
-  <si>
     <t>getText</t>
   </si>
   <si>
@@ -293,9 +290,6 @@
     <t>TITLE matches : oneView</t>
   </si>
   <si>
-    <t>Typed Automationuser into USERNAME_TEXTBOX text box</t>
-  </si>
-  <si>
     <t>Typed Interface1 into PASSWORD_TEXTBOX text box</t>
   </si>
   <si>
@@ -305,502 +299,460 @@
     <t>Waiting for 18000 millisecond  text box to be present</t>
   </si>
   <si>
+    <t>Waiting for 2000 millisecond  text box to be present</t>
+  </si>
+  <si>
+    <t>clicked on USER_DROPDOWN</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>ChangeCompany</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>SETTINGS_LINK</t>
+  </si>
+  <si>
+    <t>Vishak.Nair</t>
+  </si>
+  <si>
+    <t>CHANGECOMPANY_LINK</t>
+  </si>
+  <si>
+    <t>Typed Vishak.Nair into USERNAME_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Settings </t>
+  </si>
+  <si>
+    <t>USER_SETTINGS</t>
+  </si>
+  <si>
+    <t>verifyElement</t>
+  </si>
+  <si>
+    <t>OLD_PASSWORD</t>
+  </si>
+  <si>
+    <t>NEW_PASSWORD</t>
+  </si>
+  <si>
+    <t>CONFIRM_PASSWORD</t>
+  </si>
+  <si>
+    <t>UPDATE_BUTTON</t>
+  </si>
+  <si>
+    <t>Interface2</t>
+  </si>
+  <si>
+    <t>USER_NAME_SETTINGS</t>
+  </si>
+  <si>
+    <t>LOGIN_ERRORMSG</t>
+  </si>
+  <si>
+    <t>Login Error: The username/password you provided were incorrect.</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>ADMIN_LINK</t>
+  </si>
+  <si>
+    <t>getTextContent</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>clicked on SETTINGS_LINK</t>
+  </si>
+  <si>
+    <t>Element present : USER_SETTINGS</t>
+  </si>
+  <si>
+    <t>Element present : vishak.nair</t>
+  </si>
+  <si>
+    <t>Typed Interface1 into OLD_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Typed Interface2 into NEW_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Typed Interface2 into CONFIRM_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>clicked on UPDATE_BUTTON</t>
+  </si>
+  <si>
+    <t>clicked on LOGOUT_LINK</t>
+  </si>
+  <si>
+    <t>clear the field  PASSWORD_TEXTBOX</t>
+  </si>
+  <si>
+    <t>Typed Interface2 into PASSWORD_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t>Element present : Login Error: The username/password you provided were incorrect.</t>
+  </si>
+  <si>
+    <t>CREATE_NEWUSER</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>CREATEUSER_USERNAME</t>
+  </si>
+  <si>
+    <t>AutomationUser</t>
+  </si>
+  <si>
+    <t>Create User</t>
+  </si>
+  <si>
+    <t>CREATEUSER_TITLE</t>
+  </si>
+  <si>
+    <t>CREATEUSER_EMAIL</t>
+  </si>
+  <si>
+    <t>CREATEUSER_PASSWORD</t>
+  </si>
+  <si>
+    <t>CREATEUSER_CONFIRMPASSWORD</t>
+  </si>
+  <si>
+    <t>nandini.rajaram@interfacesys.com</t>
+  </si>
+  <si>
+    <t>Auto123</t>
+  </si>
+  <si>
+    <t>CREATEUSER_SUBMIT</t>
+  </si>
+  <si>
+    <t>USERCREATION_SUCCESSMESSAGE</t>
+  </si>
+  <si>
+    <t>User Automation User created successfully.</t>
+  </si>
+  <si>
+    <t>CREATEUSERMENU_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>TS33</t>
+  </si>
+  <si>
+    <t>TS34</t>
+  </si>
+  <si>
+    <t>TS35</t>
+  </si>
+  <si>
+    <t>TS36</t>
+  </si>
+  <si>
+    <t>TS37</t>
+  </si>
+  <si>
+    <t>FILTER_USERNAME</t>
+  </si>
+  <si>
+    <t>TS38</t>
+  </si>
+  <si>
+    <t>FILTER_BUTTON</t>
+  </si>
+  <si>
+    <t>partialLinkText</t>
+  </si>
+  <si>
+    <t>TS39</t>
+  </si>
+  <si>
+    <t>TS40</t>
+  </si>
+  <si>
+    <t>TS41</t>
+  </si>
+  <si>
+    <t>TS42</t>
+  </si>
+  <si>
+    <t>TS43</t>
+  </si>
+  <si>
+    <t>TS44</t>
+  </si>
+  <si>
+    <t>TS45</t>
+  </si>
+  <si>
+    <t>TS46</t>
+  </si>
+  <si>
+    <t>TS47</t>
+  </si>
+  <si>
+    <t>TS48</t>
+  </si>
+  <si>
+    <t>TS49</t>
+  </si>
+  <si>
+    <t>TS50</t>
+  </si>
+  <si>
+    <t>TS51</t>
+  </si>
+  <si>
+    <t>searchElement</t>
+  </si>
+  <si>
+    <t>FILTER_TABLE</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>TS52</t>
+  </si>
+  <si>
+    <t>EDITAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>TS53</t>
+  </si>
+  <si>
+    <t>TS54</t>
+  </si>
+  <si>
+    <t>EDITUSER_TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit User </t>
+  </si>
+  <si>
+    <t>TS55</t>
+  </si>
+  <si>
+    <t>ADMINROLE_CHECKBOX</t>
+  </si>
+  <si>
+    <t>TS56</t>
+  </si>
+  <si>
+    <t>UPDATEBUTTON_EDITSCREEN</t>
+  </si>
+  <si>
+    <t>TS57</t>
+  </si>
+  <si>
+    <t>TS58</t>
+  </si>
+  <si>
+    <t>EDITSCREEN_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>TS59</t>
+  </si>
+  <si>
+    <t>TS60</t>
+  </si>
+  <si>
+    <t>DELETEAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>accept alert</t>
+  </si>
+  <si>
+    <t>TS61</t>
+  </si>
+  <si>
+    <t>TS62</t>
+  </si>
+  <si>
+    <t>clicked on ADMIN_LINK</t>
+  </si>
+  <si>
+    <t>clicked on CREATE_NEWUSER</t>
+  </si>
+  <si>
+    <t>Waiting for 1000 millisecond  text box to be present</t>
+  </si>
+  <si>
+    <t>Element present : CREATEUSER_TITLE</t>
+  </si>
+  <si>
+    <t>Typed AutomationUser into CREATEUSER_USERNAME text box</t>
+  </si>
+  <si>
+    <t>Typed nandini.rajaram@interfacesys.com into CREATEUSER_EMAIL text box</t>
+  </si>
+  <si>
+    <t>Typed Auto123 into CREATEUSER_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Typed Auto123 into CREATEUSER_CONFIRMPASSWORD text box</t>
+  </si>
+  <si>
+    <t>clicked on CREATEUSER_SUBMIT</t>
+  </si>
+  <si>
+    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                 User AutomationUser created successfully.</t>
+  </si>
+  <si>
+    <t>clicked on CREATEUSERMENU_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>Typed AutomationUser into USERNAME_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t>Typed Auto123 into PASSWORD_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t>Typed AutomationUser into FILTER_USERNAME text box</t>
+  </si>
+  <si>
+    <t>clicked on FILTER_BUTTON</t>
+  </si>
+  <si>
+    <t>Element FILTER_TABLE not found</t>
+  </si>
+  <si>
+    <t>clicked on EDITAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>Element present : Edit User</t>
+  </si>
+  <si>
+    <t>clicked on ADMINROLE_CHECKBOX</t>
+  </si>
+  <si>
+    <t>clicked on UPDATEBUTTON_EDITSCREEN</t>
+  </si>
+  <si>
+    <t>clicked on EDITSCREEN_CLOSEBUTTON</t>
+  </si>
+  <si>
+    <t>clicked on DELETEAUTOMATIONUSER</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>25000</t>
+  </si>
+  <si>
+    <t>COMPANY_DROPDOWN</t>
+  </si>
+  <si>
+    <t>DOLLAR EXPRESS</t>
+  </si>
+  <si>
+    <t>ChangeCompany_button</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>Waiting for 5000 millisecond  text box to be present</t>
+  </si>
+  <si>
+    <t>Typed Interface2 into OLD_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Typed Interface1 into NEW_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Typed Interface1 into CONFIRM_PASSWORD text box</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>SEARCH_FIELD</t>
+  </si>
+  <si>
+    <t>SEARCHRESULT</t>
+  </si>
+  <si>
+    <t>1442</t>
+  </si>
+  <si>
+    <t>callSearchObject</t>
+  </si>
+  <si>
+    <t>Typed 1442 into SEARCH_FIELD text box</t>
+  </si>
+  <si>
+    <t>clicked on SEARCHRESULT</t>
+  </si>
+  <si>
+    <t>Verified the address</t>
+  </si>
+  <si>
+    <t>ONEVIEWLOGO</t>
+  </si>
+  <si>
+    <t>LogoVerification</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>http://oneviewdev.interfacesys.com/Main.aspx</t>
+  </si>
+  <si>
+    <t>verifyCurrentURL</t>
+  </si>
+  <si>
+    <t>clicked on ONEVIEWLOGO</t>
+  </si>
+  <si>
+    <t>Navigated to the Home page</t>
+  </si>
+  <si>
+    <t>Element USERNAME_TEXTBOX not found</t>
+  </si>
+  <si>
+    <t>Element PASSWORD_TEXTBOX not found</t>
+  </si>
+  <si>
+    <t>Element SUBMIT_BUTTON not found</t>
+  </si>
+  <si>
+    <t>faiz.dani</t>
+  </si>
+  <si>
+    <t>Element DES_TEXTBOX not found</t>
+  </si>
+  <si>
+    <t>Typed faiz.dani into USERNAME_TEXTBOX text box</t>
+  </si>
+  <si>
+    <t>Element SUBMITCASE_BUTTON not found</t>
+  </si>
+  <si>
     <t>Waiting for 9000 millisecond  text box to be present</t>
   </si>
   <si>
-    <t>Waiting for 2000 millisecond  text box to be present</t>
-  </si>
-  <si>
-    <t>Typed smathew@suyati.com into EMAIL_TEXTBOX text box</t>
-  </si>
-  <si>
-    <t>Element present :</t>
-  </si>
-  <si>
-    <t>clicked on CLOSEPOPUP_LINK</t>
-  </si>
-  <si>
-    <t>clicked on USER_DROPDOWN</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>Element SUBMITCASE_BUTTON not found</t>
-  </si>
-  <si>
-    <t>Element CASESEARCH_TEXTBOX not found</t>
-  </si>
-  <si>
-    <t>Element SITE_LINK not found</t>
-  </si>
-  <si>
-    <t>Element DES_TEXTBOX not found</t>
-  </si>
-  <si>
-    <t>Element SYSTEM_DROPDOWN not found</t>
-  </si>
-  <si>
-    <t>Element PREMISEHOUR_TEXTBOX not found</t>
-  </si>
-  <si>
-    <t>Element FULLNAME_TEXTBOX not found</t>
-  </si>
-  <si>
-    <t>Element CONTACT_TEXTBOX not found</t>
-  </si>
-  <si>
-    <t>Element STARTTIME_TEXTBOX not found</t>
-  </si>
-  <si>
-    <t>Element PREFERREDHOURS_DROPDOWN not found</t>
-  </si>
-  <si>
-    <t>Element ALTERNATEPHONE_TEXTBOX not found</t>
-  </si>
-  <si>
-    <t>Element PRIORITY_CHECKBOX not found</t>
-  </si>
-  <si>
-    <t>Element SUBMITACASE_LINK not found</t>
-  </si>
-  <si>
-    <t>ChangeCompany</t>
-  </si>
-  <si>
-    <t>Settings</t>
-  </si>
-  <si>
-    <t>SETTINGS_LINK</t>
-  </si>
-  <si>
-    <t>Vishak.Nair</t>
-  </si>
-  <si>
-    <t>CHANGECOMPANY_LINK</t>
-  </si>
-  <si>
-    <t>Typed Vishak.Nair into USERNAME_TEXTBOX text box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Settings </t>
-  </si>
-  <si>
-    <t>USER_SETTINGS</t>
-  </si>
-  <si>
-    <t>verifyElement</t>
-  </si>
-  <si>
-    <t>OLD_PASSWORD</t>
-  </si>
-  <si>
-    <t>NEW_PASSWORD</t>
-  </si>
-  <si>
-    <t>CONFIRM_PASSWORD</t>
-  </si>
-  <si>
-    <t>UPDATE_BUTTON</t>
-  </si>
-  <si>
-    <t>Interface2</t>
-  </si>
-  <si>
-    <t>USER_NAME_SETTINGS</t>
-  </si>
-  <si>
-    <t>LOGIN_ERRORMSG</t>
-  </si>
-  <si>
-    <t>Login Error: The username/password you provided were incorrect.</t>
-  </si>
-  <si>
-    <t>clear</t>
-  </si>
-  <si>
-    <t>ADMIN_LINK</t>
-  </si>
-  <si>
-    <t>getTextContent</t>
-  </si>
-  <si>
-    <t>Administration</t>
-  </si>
-  <si>
-    <t>clicked on SETTINGS_LINK</t>
-  </si>
-  <si>
-    <t>Element present : USER_SETTINGS</t>
-  </si>
-  <si>
-    <t>Element present : vishak.nair</t>
-  </si>
-  <si>
-    <t>Typed Interface1 into OLD_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Typed Interface2 into NEW_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Typed Interface2 into CONFIRM_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>clicked on UPDATE_BUTTON</t>
-  </si>
-  <si>
-    <t>clicked on LOGOUT_LINK</t>
-  </si>
-  <si>
-    <t>clear the field  PASSWORD_TEXTBOX</t>
-  </si>
-  <si>
-    <t>Typed Interface2 into PASSWORD_TEXTBOX text box</t>
-  </si>
-  <si>
-    <t>Element present : Login Error: The username/password you provided were incorrect.</t>
-  </si>
-  <si>
-    <t>CREATE_NEWUSER</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>CREATEUSER_USERNAME</t>
-  </si>
-  <si>
-    <t>AutomationUser</t>
-  </si>
-  <si>
-    <t>Create User</t>
-  </si>
-  <si>
-    <t>CREATEUSER_TITLE</t>
-  </si>
-  <si>
-    <t>CREATEUSER_EMAIL</t>
-  </si>
-  <si>
-    <t>CREATEUSER_PASSWORD</t>
-  </si>
-  <si>
-    <t>CREATEUSER_CONFIRMPASSWORD</t>
-  </si>
-  <si>
-    <t>nandini.rajaram@interfacesys.com</t>
-  </si>
-  <si>
-    <t>Auto123</t>
-  </si>
-  <si>
-    <t>CREATEUSER_SUBMIT</t>
-  </si>
-  <si>
-    <t>USERCREATION_SUCCESSMESSAGE</t>
-  </si>
-  <si>
-    <t>User Automation User created successfully.</t>
-  </si>
-  <si>
-    <t>CREATEUSERMENU_CLOSEBUTTON</t>
-  </si>
-  <si>
-    <t>TS33</t>
-  </si>
-  <si>
-    <t>TS34</t>
-  </si>
-  <si>
-    <t>TS35</t>
-  </si>
-  <si>
-    <t>TS36</t>
-  </si>
-  <si>
-    <t>TS37</t>
-  </si>
-  <si>
-    <t>FILTER_USERNAME</t>
-  </si>
-  <si>
-    <t>TS38</t>
-  </si>
-  <si>
-    <t>FILTER_BUTTON</t>
-  </si>
-  <si>
-    <t>partialLinkText</t>
-  </si>
-  <si>
-    <t>TS39</t>
-  </si>
-  <si>
-    <t>TS40</t>
-  </si>
-  <si>
-    <t>TS41</t>
-  </si>
-  <si>
-    <t>TS42</t>
-  </si>
-  <si>
-    <t>TS43</t>
-  </si>
-  <si>
-    <t>TS44</t>
-  </si>
-  <si>
-    <t>TS45</t>
-  </si>
-  <si>
-    <t>TS46</t>
-  </si>
-  <si>
-    <t>TS47</t>
-  </si>
-  <si>
-    <t>TS48</t>
-  </si>
-  <si>
-    <t>TS49</t>
-  </si>
-  <si>
-    <t>TS50</t>
-  </si>
-  <si>
-    <t>TS51</t>
-  </si>
-  <si>
-    <t>searchElement</t>
-  </si>
-  <si>
-    <t>FILTER_TABLE</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>TS52</t>
-  </si>
-  <si>
-    <t>EDITAUTOMATIONUSER</t>
-  </si>
-  <si>
-    <t>TS53</t>
-  </si>
-  <si>
-    <t>TS54</t>
-  </si>
-  <si>
-    <t>EDITUSER_TITLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edit User </t>
-  </si>
-  <si>
-    <t>TS55</t>
-  </si>
-  <si>
-    <t>ADMINROLE_CHECKBOX</t>
-  </si>
-  <si>
-    <t>TS56</t>
-  </si>
-  <si>
-    <t>UPDATEBUTTON_EDITSCREEN</t>
-  </si>
-  <si>
-    <t>TS57</t>
-  </si>
-  <si>
-    <t>TS58</t>
-  </si>
-  <si>
-    <t>EDITSCREEN_CLOSEBUTTON</t>
-  </si>
-  <si>
-    <t>TS59</t>
-  </si>
-  <si>
-    <t>TS60</t>
-  </si>
-  <si>
-    <t>DELETEAUTOMATIONUSER</t>
-  </si>
-  <si>
-    <t>accept alert</t>
-  </si>
-  <si>
-    <t>TS61</t>
-  </si>
-  <si>
-    <t>TS62</t>
-  </si>
-  <si>
-    <t>clicked on ADMIN_LINK</t>
-  </si>
-  <si>
-    <t>clicked on CREATE_NEWUSER</t>
-  </si>
-  <si>
-    <t>Waiting for 1000 millisecond  text box to be present</t>
-  </si>
-  <si>
-    <t>Element present : CREATEUSER_TITLE</t>
-  </si>
-  <si>
-    <t>Typed AutomationUser into CREATEUSER_USERNAME text box</t>
-  </si>
-  <si>
-    <t>Typed nandini.rajaram@interfacesys.com into CREATEUSER_EMAIL text box</t>
-  </si>
-  <si>
-    <t>Typed Auto123 into CREATEUSER_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Typed Auto123 into CREATEUSER_CONFIRMPASSWORD text box</t>
-  </si>
-  <si>
-    <t>clicked on CREATEUSER_SUBMIT</t>
-  </si>
-  <si>
-    <t>Element present :                                                                                     Username:                                                                     Password:                                     Confirm:                                                                                             Email:                                                                                                                                         Submit                                                                                                                                                 User AutomationUser created successfully.</t>
-  </si>
-  <si>
-    <t>clicked on CREATEUSERMENU_CLOSEBUTTON</t>
-  </si>
-  <si>
-    <t>Typed AutomationUser into USERNAME_TEXTBOX text box</t>
-  </si>
-  <si>
-    <t>Typed Auto123 into PASSWORD_TEXTBOX text box</t>
-  </si>
-  <si>
-    <t>Typed AutomationUser into FILTER_USERNAME text box</t>
-  </si>
-  <si>
-    <t>clicked on FILTER_BUTTON</t>
-  </si>
-  <si>
-    <t>Element FILTER_TABLE not found</t>
-  </si>
-  <si>
-    <t>clicked on EDITAUTOMATIONUSER</t>
-  </si>
-  <si>
-    <t>Element present : Edit User</t>
-  </si>
-  <si>
-    <t>clicked on ADMINROLE_CHECKBOX</t>
-  </si>
-  <si>
-    <t>clicked on UPDATEBUTTON_EDITSCREEN</t>
-  </si>
-  <si>
-    <t>clicked on EDITSCREEN_CLOSEBUTTON</t>
-  </si>
-  <si>
-    <t>clicked on DELETEAUTOMATIONUSER</t>
-  </si>
-  <si>
-    <t>Accepted</t>
-  </si>
-  <si>
-    <t>25000</t>
-  </si>
-  <si>
-    <t>COMPANY_DROPDOWN</t>
-  </si>
-  <si>
-    <t>DOLLAR EXPRESS</t>
-  </si>
-  <si>
-    <t>ChangeCompany_button</t>
-  </si>
-  <si>
-    <t>10000</t>
-  </si>
-  <si>
     <t>Waiting for 25000 millisecond  text box to be present</t>
   </si>
   <si>
     <t>clicked on CHANGECOMPANY_LINK</t>
   </si>
   <si>
-    <t>Waiting for 5000 millisecond  text box to be present</t>
-  </si>
-  <si>
-    <t>clicked on ChangeCompany_button</t>
-  </si>
-  <si>
     <t>Waiting for 10000 millisecond  text box to be present</t>
-  </si>
-  <si>
-    <t>Element COMPANY_DROPDOWN not found</t>
-  </si>
-  <si>
-    <t>Typed Interface2 into OLD_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Typed Interface1 into NEW_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Typed Interface1 into CONFIRM_PASSWORD text box</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>SEARCH_FIELD</t>
-  </si>
-  <si>
-    <t>SEARCHRESULT</t>
-  </si>
-  <si>
-    <t>1442</t>
-  </si>
-  <si>
-    <t>callSearchObject</t>
-  </si>
-  <si>
-    <t>Typed 1442 into SEARCH_FIELD text box</t>
-  </si>
-  <si>
-    <t>clicked on SEARCHRESULT</t>
-  </si>
-  <si>
-    <t>Verified the address</t>
-  </si>
-  <si>
-    <t>ONEVIEWLOGO</t>
-  </si>
-  <si>
-    <t>LogoVerification</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>http://oneviewdev.interfacesys.com/Main.aspx</t>
-  </si>
-  <si>
-    <t>verifyCurrentURL</t>
-  </si>
-  <si>
-    <t>clicked on ONEVIEWLOGO</t>
-  </si>
-  <si>
-    <t>Navigated to the Home page</t>
-  </si>
-  <si>
-    <t>Element USERNAME_TEXTBOX not found</t>
-  </si>
-  <si>
-    <t>Element PASSWORD_TEXTBOX not found</t>
-  </si>
-  <si>
-    <t>Element SUBMIT_BUTTON not found</t>
   </si>
 </sst>
 </file>
@@ -1193,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,20 +1176,20 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
         <v>75</v>
@@ -1245,7 +1197,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
         <v>75</v>
@@ -1253,18 +1205,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="B7" t="s">
-        <v>252</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="B8" t="s">
-        <v>252</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1333,7 +1285,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1448,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544B4CF8-F8F5-43C8-B474-A7437C7BA17B}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,7 +1410,7 @@
     <col min="5" max="5" width="20.28515625" hidden="false" bestFit="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1475,7 +1427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1488,13 +1440,13 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1508,16 +1460,16 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>80</v>
+        <v>236</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1534,13 +1486,13 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -1555,13 +1507,13 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1574,13 +1526,13 @@
         <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1595,13 +1547,13 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1614,13 +1566,13 @@
         <v>77</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1636,14 +1588,8 @@
       <c r="E9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F9" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1655,14 +1601,8 @@
       <c r="E10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F10" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
@@ -1676,14 +1616,8 @@
         <v>10</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" t="s">
-        <v>100</v>
-      </c>
-      <c r="G11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
@@ -1696,13 +1630,13 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -1719,13 +1653,13 @@
         <v>35</v>
       </c>
       <c r="F13" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -1737,14 +1671,8 @@
       <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F14" t="s">
-        <v>88</v>
-      </c>
-      <c r="G14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -1760,14 +1688,8 @@
       <c r="E15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F15" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -1779,12 +1701,6 @@
       <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1802,12 +1718,6 @@
       <c r="E17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F17" t="s">
-        <v>100</v>
-      </c>
-      <c r="G17" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1825,12 +1735,8 @@
       <c r="E18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F18" t="s">
-        <v>100</v>
-      </c>
-      <c r="G18" t="s">
-        <v>107</v>
-      </c>
+      <c r="F18"/>
+      <c r="G18"/>
     </row>
     <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1848,12 +1754,8 @@
       <c r="E19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F19" t="s">
-        <v>100</v>
-      </c>
-      <c r="G19" t="s">
-        <v>108</v>
-      </c>
+      <c r="F19"/>
+      <c r="G19"/>
     </row>
     <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1871,12 +1773,8 @@
       <c r="E20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G20" t="s">
-        <v>109</v>
-      </c>
+      <c r="F20"/>
+      <c r="G20"/>
     </row>
     <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1894,12 +1792,8 @@
       <c r="E21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F21" t="s">
-        <v>100</v>
-      </c>
-      <c r="G21" t="s">
-        <v>110</v>
-      </c>
+      <c r="F21"/>
+      <c r="G21"/>
     </row>
     <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1917,12 +1811,8 @@
       <c r="E22" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F22" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" t="s">
-        <v>96</v>
-      </c>
+      <c r="F22"/>
+      <c r="G22"/>
     </row>
     <row r="23" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1940,12 +1830,8 @@
       <c r="E23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" t="s">
-        <v>111</v>
-      </c>
+      <c r="F23"/>
+      <c r="G23"/>
     </row>
     <row r="24" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1961,12 +1847,8 @@
         <v>10</v>
       </c>
       <c r="E24" s="2"/>
-      <c r="F24" t="s">
-        <v>100</v>
-      </c>
-      <c r="G24" t="s">
-        <v>112</v>
-      </c>
+      <c r="F24"/>
+      <c r="G24"/>
     </row>
     <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1982,12 +1864,8 @@
         <v>10</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25" t="s">
-        <v>100</v>
-      </c>
-      <c r="G25" t="s">
-        <v>113</v>
-      </c>
+      <c r="F25"/>
+      <c r="G25"/>
     </row>
     <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -2001,12 +1879,8 @@
       <c r="E26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F26" t="s">
-        <v>88</v>
-      </c>
-      <c r="G26" t="s">
-        <v>94</v>
-      </c>
+      <c r="F26"/>
+      <c r="G26"/>
     </row>
     <row r="27" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -2016,18 +1890,14 @@
         <v>9</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" t="s">
-        <v>88</v>
-      </c>
-      <c r="G27" t="s">
-        <v>97</v>
-      </c>
+      <c r="F27"/>
+      <c r="G27"/>
     </row>
     <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -2041,12 +1911,8 @@
       <c r="E28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F28" t="s">
-        <v>88</v>
-      </c>
-      <c r="G28" t="s">
-        <v>95</v>
-      </c>
+      <c r="F28"/>
+      <c r="G28"/>
     </row>
     <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -2056,22 +1922,18 @@
         <v>11</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" t="s">
-        <v>88</v>
-      </c>
-      <c r="G29" t="s">
-        <v>98</v>
-      </c>
+      <c r="F29"/>
+      <c r="G29"/>
     </row>
     <row r="30" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2081,16 +1943,12 @@
       <c r="E30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F30" t="s">
-        <v>88</v>
-      </c>
-      <c r="G30" t="s">
-        <v>95</v>
-      </c>
+      <c r="F30"/>
+      <c r="G30"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>11</v>
@@ -2102,16 +1960,10 @@
         <v>10</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2121,16 +1973,10 @@
       <c r="E32" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F32" t="s">
-        <v>88</v>
-      </c>
-      <c r="G32" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>13</v>
@@ -2145,7 +1991,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E22" r:id="rId30" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
+    <hyperlink ref="E22" r:id="rId58" xr:uid="{3489C5A6-4810-4125-83C6-BFA8F960F163}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -2154,10 +2000,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C24C14-A866-4140-B688-97F68D23BE6D}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2167,7 +2013,7 @@
     <col min="5" max="5" width="15.85546875" hidden="false" bestFit="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2184,7 +2030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2197,13 +2043,13 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2217,16 +2063,16 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>236</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="G3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2243,13 +2089,13 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -2264,13 +2110,13 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -2280,16 +2126,16 @@
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -2297,20 +2143,20 @@
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -2320,16 +2166,10 @@
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -2337,22 +2177,16 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="F9" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -2362,16 +2196,10 @@
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F10" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
@@ -2379,20 +2207,14 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
@@ -2402,16 +2224,16 @@
         <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -2424,13 +2246,13 @@
         <v>26</v>
       </c>
       <c r="F13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -2445,13 +2267,13 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -2464,13 +2286,13 @@
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -2485,10 +2307,10 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G16" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2544,10 +2366,10 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" t="s">
         <v>88</v>
-      </c>
-      <c r="G2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2564,13 +2386,13 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2590,10 +2412,10 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2611,10 +2433,10 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2630,10 +2452,10 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2651,10 +2473,10 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2670,10 +2492,10 @@
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2684,17 +2506,17 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2710,10 +2532,10 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2724,17 +2546,17 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2747,13 +2569,13 @@
         <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2764,19 +2586,19 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="F13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G13" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2787,19 +2609,19 @@
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="F14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2810,19 +2632,19 @@
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2833,19 +2655,19 @@
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="F16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G16" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2856,19 +2678,19 @@
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="F17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G17" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2879,17 +2701,17 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G18" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2900,19 +2722,19 @@
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="F19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G19" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2923,22 +2745,22 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G20" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>11</v>
@@ -2951,15 +2773,15 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G21" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2970,15 +2792,15 @@
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G22" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>13</v>
@@ -2991,15 +2813,15 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G23" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -3010,15 +2832,15 @@
         <v>26</v>
       </c>
       <c r="F24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" t="s">
         <v>88</v>
-      </c>
-      <c r="G24" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -3030,18 +2852,18 @@
         <v>6</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="F25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G25" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>9</v>
@@ -3053,18 +2875,18 @@
         <v>6</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="F26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G26" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>9</v>
@@ -3077,15 +2899,15 @@
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3096,15 +2918,15 @@
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G28" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>11</v>
@@ -3117,15 +2939,15 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G29" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3136,15 +2958,15 @@
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G30" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
@@ -3157,15 +2979,15 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G31" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3176,15 +2998,15 @@
         <v>26</v>
       </c>
       <c r="F32" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" t="s">
         <v>88</v>
-      </c>
-      <c r="G32" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>9</v>
@@ -3196,18 +3018,18 @@
         <v>6</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>9</v>
@@ -3222,15 +3044,15 @@
         <v>27</v>
       </c>
       <c r="F34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>9</v>
@@ -3243,15 +3065,15 @@
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3262,15 +3084,15 @@
         <v>25</v>
       </c>
       <c r="F36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>11</v>
@@ -3283,15 +3105,15 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G37" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3302,36 +3124,36 @@
         <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G38" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G39" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3342,103 +3164,103 @@
         <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G40" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="F41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G41" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G42" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="F43" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G43" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G44" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3449,80 +3271,80 @@
         <v>25</v>
       </c>
       <c r="F45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G45" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="F46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G46" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G47" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G48" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3533,36 +3355,36 @@
         <v>25</v>
       </c>
       <c r="F49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G49" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G50" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3573,36 +3395,36 @@
         <v>25</v>
       </c>
       <c r="F51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G51" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G52" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3613,32 +3435,32 @@
         <v>25</v>
       </c>
       <c r="F53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G53" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G54" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>11</v>
@@ -3651,15 +3473,15 @@
       </c>
       <c r="E55" s="1"/>
       <c r="F55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G55" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3670,15 +3492,15 @@
         <v>25</v>
       </c>
       <c r="F56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G56" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>13</v>
@@ -3691,15 +3513,15 @@
       </c>
       <c r="E57" s="1"/>
       <c r="F57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G57" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3710,15 +3532,15 @@
         <v>26</v>
       </c>
       <c r="F58" t="s">
+        <v>87</v>
+      </c>
+      <c r="G58" t="s">
         <v>88</v>
-      </c>
-      <c r="G58" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>9</v>
@@ -3730,18 +3552,18 @@
         <v>6</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="F59" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G59" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>9</v>
@@ -3753,18 +3575,18 @@
         <v>6</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="F60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G60" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>9</v>
@@ -3777,10 +3599,10 @@
       </c>
       <c r="E61" s="2"/>
       <c r="F61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G61" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3791,24 +3613,24 @@
         <v>11</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="F62" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G62" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId30" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
+    <hyperlink ref="E15" r:id="rId58" xr:uid="{D816654D-A10D-47EB-9214-38410769A695}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
@@ -3861,10 +3683,10 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" t="s">
         <v>88</v>
-      </c>
-      <c r="G2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3881,13 +3703,13 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3907,10 +3729,10 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3928,10 +3750,10 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3947,10 +3769,10 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3968,10 +3790,10 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3987,10 +3809,10 @@
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4001,17 +3823,17 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4027,10 +3849,10 @@
         <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4041,19 +3863,19 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="F11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4064,19 +3886,19 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -4087,7 +3909,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -4096,10 +3918,10 @@
         <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G13" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4110,19 +3932,19 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="F14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4133,19 +3955,19 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4156,17 +3978,17 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G16" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -4184,10 +4006,10 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G17" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -4203,10 +4025,10 @@
         <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -4224,10 +4046,10 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G19" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -4243,10 +4065,10 @@
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -4262,10 +4084,10 @@
         <v>26</v>
       </c>
       <c r="F21" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" t="s">
         <v>88</v>
-      </c>
-      <c r="G21" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -4282,13 +4104,13 @@
         <v>6</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G22" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -4308,10 +4130,10 @@
         <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -4329,10 +4151,10 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -4343,19 +4165,19 @@
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="F25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G25" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -4369,14 +4191,14 @@
         <v>18</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G26" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -4393,13 +4215,13 @@
         <v>6</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="F27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G27" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4417,10 +4239,10 @@
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -4436,15 +4258,15 @@
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G29" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>11</v>
@@ -4457,36 +4279,36 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G30" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G31" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -4497,90 +4319,90 @@
         <v>76</v>
       </c>
       <c r="F32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="F33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G34" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="F35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G35" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>6</v>
@@ -4589,21 +4411,21 @@
         <v>27</v>
       </c>
       <c r="F36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G36" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>6</v>
@@ -4612,31 +4434,31 @@
         <v>27</v>
       </c>
       <c r="F37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G37" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G38" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -4654,10 +4476,10 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G39" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -4673,10 +4495,10 @@
         <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G40" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -4694,10 +4516,10 @@
       </c>
       <c r="E41" s="1"/>
       <c r="F41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G41" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4752,10 +4574,10 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" t="s">
         <v>88</v>
-      </c>
-      <c r="G2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4772,13 +4594,13 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4798,10 +4620,10 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4819,10 +4641,10 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -4838,10 +4660,10 @@
         <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -4852,19 +4674,19 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="F7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -4877,13 +4699,13 @@
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4894,17 +4716,17 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4920,10 +4742,10 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4933,14 +4755,14 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -5010,10 +4832,10 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" t="s">
         <v>88</v>
-      </c>
-      <c r="G2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -5030,13 +4852,13 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G3" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -5056,10 +4878,10 @@
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G4" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -5077,10 +4899,10 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G5" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -5096,10 +4918,10 @@
         <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -5110,19 +4932,19 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="F7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -5135,13 +4957,13 @@
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -5152,17 +4974,17 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -5178,10 +5000,10 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -5191,14 +5013,14 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -5209,17 +5031,17 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -5229,16 +5051,16 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
       <c r="E13" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="F13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G13" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>